<commit_message>
KIBON-2265: Save results in correct field in BGResult
</commit_message>
<xml_diff>
--- a/ebegu-server/src/test/java/ch/dvbern/ebegu/rechner/BG_Rechner_Luzern_0.1_Stand_Dez21.xlsx
+++ b/ebegu-server/src/test/java/ch/dvbern/ebegu/rechner/BG_Rechner_Luzern_0.1_Stand_Dez21.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ebegu\ebegu-server\src\test\java\ch\dvbern\ebegu\rechner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCE1A55-2E17-4F7A-B37D-875FF5288313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FF3834-A4B5-45D8-B01B-D6042E2298F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kita" sheetId="8" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="62">
   <si>
     <t>Minimaltarif</t>
   </si>
@@ -210,6 +210,18 @@
   </si>
   <si>
     <t>Monatliche Vollkosten (gekürzt)</t>
+  </si>
+  <si>
+    <t>Abzüglich minimaler Elternbeitrag</t>
+  </si>
+  <si>
+    <t>An Institution/Eltern überwiesener Betrag</t>
+  </si>
+  <si>
+    <t>Gutscheinbetrag gemäss Formel in CHF  (VergOhneBeruecksichtigungVollkosten)</t>
+  </si>
+  <si>
+    <t>Betreuungsgutschein in CHF (VergOhneBeruecksichtigungMinimalbetrag)</t>
   </si>
 </sst>
 </file>
@@ -315,7 +327,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -365,13 +377,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -460,15 +501,89 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
-    <xf numFmtId="9" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="1" fontId="5" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="6" borderId="5" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="6" borderId="6" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="8" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Eingabe" xfId="2" builtinId="20"/>
@@ -751,16 +866,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O56"/>
+  <dimension ref="A1:T56"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="T50" sqref="T50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50" style="11" customWidth="1"/>
-    <col min="2" max="2" width="4.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="11" customWidth="1"/>
     <col min="4" max="4" width="3" style="11" customWidth="1"/>
     <col min="5" max="5" width="16" style="11" customWidth="1"/>
@@ -769,25 +884,33 @@
     <col min="8" max="8" width="3" style="11" customWidth="1"/>
     <col min="9" max="9" width="16" style="11" customWidth="1"/>
     <col min="10" max="10" width="3" style="11" customWidth="1"/>
-    <col min="11" max="11" width="1.88671875" style="11" customWidth="1"/>
-    <col min="12" max="12" width="94.88671875" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="11.44140625" style="11"/>
+    <col min="11" max="11" width="16" style="11" customWidth="1"/>
+    <col min="12" max="12" width="3" style="23" customWidth="1"/>
+    <col min="13" max="13" width="0.42578125" style="11" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" style="11" customWidth="1"/>
+    <col min="15" max="15" width="3" style="11" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" customWidth="1"/>
+    <col min="17" max="17" width="3.5703125" style="11" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" style="11" customWidth="1"/>
+    <col min="19" max="19" width="3.7109375" style="11" customWidth="1"/>
+    <col min="20" max="20" width="94.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="11.42578125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="49"/>
     </row>
-    <row r="3" spans="1:12" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C4" s="13" t="s">
         <v>55</v>
       </c>
@@ -801,19 +924,44 @@
         <v>2</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="14">
-        <v>1</v>
+        <v>55</v>
+      </c>
+      <c r="H4" s="57">
+        <v>3</v>
       </c>
       <c r="I4" s="13" t="s">
         <v>1</v>
       </c>
       <c r="J4" s="14">
+        <v>1</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="63">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="63"/>
+      <c r="N4" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="63">
+        <v>3</v>
+      </c>
+      <c r="P4" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="90">
+        <v>4</v>
+      </c>
+      <c r="R4" s="63" t="s">
+        <v>1</v>
+      </c>
+      <c r="S4" s="63">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>46</v>
       </c>
@@ -823,11 +971,20 @@
       <c r="E5" s="18"/>
       <c r="F5" s="20"/>
       <c r="G5" s="18"/>
-      <c r="H5" s="19"/>
+      <c r="H5" s="20"/>
       <c r="I5" s="18"/>
       <c r="J5" s="19"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K5" s="18"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="64"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="64"/>
+      <c r="P5" s="79"/>
+      <c r="Q5" s="91"/>
+      <c r="R5" s="64"/>
+      <c r="S5" s="64"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
         <v>45</v>
       </c>
@@ -843,16 +1000,33 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="4">
-        <v>1600</v>
+        <v>2080</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="4">
         <v>1600</v>
       </c>
       <c r="J6" s="5"/>
-      <c r="L6" s="22"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K6" s="4">
+        <v>1600</v>
+      </c>
+      <c r="L6" s="65"/>
+      <c r="M6" s="65"/>
+      <c r="N6" s="4">
+        <v>1600</v>
+      </c>
+      <c r="O6" s="65"/>
+      <c r="P6" s="80">
+        <v>1600</v>
+      </c>
+      <c r="Q6" s="92"/>
+      <c r="R6" s="65">
+        <v>1600</v>
+      </c>
+      <c r="S6" s="65"/>
+      <c r="T6" s="22"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
         <v>13</v>
       </c>
@@ -866,23 +1040,39 @@
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="6">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="6">
         <v>0.6</v>
       </c>
       <c r="J7" s="7"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="24"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K7" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="L7" s="66"/>
+      <c r="M7" s="66"/>
+      <c r="N7" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="O7" s="66"/>
+      <c r="P7" s="81">
+        <v>0.6</v>
+      </c>
+      <c r="Q7" s="93"/>
+      <c r="R7" s="66">
+        <v>0.5</v>
+      </c>
+      <c r="S7" s="66"/>
+      <c r="T7" s="24"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="6">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="6">
@@ -890,17 +1080,33 @@
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="6">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="6">
         <v>0.6</v>
       </c>
       <c r="J8" s="7"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="24"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K8" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="L8" s="66"/>
+      <c r="M8" s="66"/>
+      <c r="N8" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="O8" s="66"/>
+      <c r="P8" s="81">
+        <v>0.4</v>
+      </c>
+      <c r="Q8" s="93"/>
+      <c r="R8" s="66">
+        <v>0.4</v>
+      </c>
+      <c r="S8" s="66"/>
+      <c r="T8" s="24"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
         <v>8</v>
       </c>
@@ -915,16 +1121,33 @@
         <v>80000</v>
       </c>
       <c r="F9" s="9"/>
-      <c r="G9" s="4">
+      <c r="G9" s="8">
+        <v>126000</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="4">
         <v>120000</v>
       </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="4">
+      <c r="J9" s="5"/>
+      <c r="K9" s="4">
         <v>125001</v>
       </c>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L9" s="65"/>
+      <c r="M9" s="65"/>
+      <c r="N9" s="4">
+        <v>48000</v>
+      </c>
+      <c r="O9" s="65"/>
+      <c r="P9" s="80">
+        <v>48000</v>
+      </c>
+      <c r="Q9" s="92"/>
+      <c r="R9" s="65">
+        <v>52000</v>
+      </c>
+      <c r="S9" s="65"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
         <v>51</v>
       </c>
@@ -939,16 +1162,33 @@
         <v>0</v>
       </c>
       <c r="F10" s="9"/>
-      <c r="G10" s="4">
-        <v>0</v>
-      </c>
-      <c r="H10" s="5"/>
+      <c r="G10" s="8">
+        <v>0</v>
+      </c>
+      <c r="H10" s="9"/>
       <c r="I10" s="4">
         <v>0</v>
       </c>
       <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K10" s="4">
+        <v>0</v>
+      </c>
+      <c r="L10" s="65"/>
+      <c r="M10" s="65"/>
+      <c r="N10" s="4">
+        <v>0</v>
+      </c>
+      <c r="O10" s="65"/>
+      <c r="P10" s="80">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="92"/>
+      <c r="R10" s="65">
+        <v>10</v>
+      </c>
+      <c r="S10" s="65"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
         <v>25</v>
       </c>
@@ -964,38 +1204,72 @@
       <c r="G11" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H11" s="5"/>
+      <c r="H11" s="9"/>
       <c r="I11" s="4" t="b">
         <v>0</v>
       </c>
       <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L11" s="65"/>
+      <c r="M11" s="65"/>
+      <c r="N11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O11" s="65"/>
+      <c r="P11" s="80" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="92"/>
+      <c r="R11" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="S11" s="65"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="21"/>
       <c r="C12" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H12" s="5"/>
+      <c r="H12" s="9"/>
       <c r="I12" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" s="5"/>
-      <c r="L12" s="11" t="s">
+      <c r="K12" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12" s="65"/>
+      <c r="M12" s="65"/>
+      <c r="N12" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O12" s="65"/>
+      <c r="P12" s="80" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="92"/>
+      <c r="R12" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="S12" s="65"/>
+      <c r="T12" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="s">
         <v>27</v>
       </c>
@@ -1011,26 +1285,52 @@
       <c r="G13" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="H13" s="5"/>
+      <c r="H13" s="9"/>
       <c r="I13" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" s="5"/>
-      <c r="L13" s="11" t="s">
+      <c r="K13" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L13" s="65"/>
+      <c r="M13" s="65"/>
+      <c r="N13" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O13" s="65"/>
+      <c r="P13" s="80" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="92"/>
+      <c r="R13" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="S13" s="65"/>
+      <c r="T13" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C14" s="13"/>
       <c r="D14" s="15"/>
       <c r="E14" s="13"/>
       <c r="F14" s="15"/>
       <c r="G14" s="13"/>
-      <c r="H14" s="14"/>
+      <c r="H14" s="15"/>
       <c r="I14" s="13"/>
       <c r="J14" s="14"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K14" s="13"/>
+      <c r="L14" s="63"/>
+      <c r="M14" s="63"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="63"/>
+      <c r="P14" s="78"/>
+      <c r="Q14" s="90"/>
+      <c r="R14" s="63"/>
+      <c r="S14" s="63"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>5</v>
       </c>
@@ -1040,11 +1340,20 @@
       <c r="E15" s="18"/>
       <c r="F15" s="20"/>
       <c r="G15" s="18"/>
-      <c r="H15" s="19"/>
+      <c r="H15" s="20"/>
       <c r="I15" s="18"/>
       <c r="J15" s="19"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K15" s="18"/>
+      <c r="L15" s="64"/>
+      <c r="M15" s="64"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="64"/>
+      <c r="P15" s="79"/>
+      <c r="Q15" s="91"/>
+      <c r="R15" s="64"/>
+      <c r="S15" s="64"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>0</v>
       </c>
@@ -1067,8 +1376,24 @@
         <v>15</v>
       </c>
       <c r="J16" s="15"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K16" s="25">
+        <v>15</v>
+      </c>
+      <c r="M16" s="23"/>
+      <c r="N16" s="25">
+        <v>15</v>
+      </c>
+      <c r="O16" s="23"/>
+      <c r="P16" s="82">
+        <v>15</v>
+      </c>
+      <c r="Q16" s="94"/>
+      <c r="R16" s="23">
+        <v>15</v>
+      </c>
+      <c r="S16" s="23"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>3</v>
       </c>
@@ -1084,15 +1409,31 @@
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="25">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="H17" s="15"/>
       <c r="I17" s="25">
         <v>130</v>
       </c>
       <c r="J17" s="15"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K17" s="25">
+        <v>130</v>
+      </c>
+      <c r="M17" s="23"/>
+      <c r="N17" s="25">
+        <v>130</v>
+      </c>
+      <c r="O17" s="23"/>
+      <c r="P17" s="82">
+        <v>130</v>
+      </c>
+      <c r="Q17" s="94"/>
+      <c r="R17" s="23">
+        <v>130</v>
+      </c>
+      <c r="S17" s="23"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>15</v>
       </c>
@@ -1115,8 +1456,24 @@
         <v>32</v>
       </c>
       <c r="J18" s="15"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K18" s="25">
+        <v>32</v>
+      </c>
+      <c r="M18" s="23"/>
+      <c r="N18" s="25">
+        <v>32</v>
+      </c>
+      <c r="O18" s="23"/>
+      <c r="P18" s="82">
+        <v>32</v>
+      </c>
+      <c r="Q18" s="94"/>
+      <c r="R18" s="23">
+        <v>32</v>
+      </c>
+      <c r="S18" s="23"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C19" s="25"/>
       <c r="D19" s="15"/>
       <c r="E19" s="25"/>
@@ -1125,8 +1482,16 @@
       <c r="H19" s="15"/>
       <c r="I19" s="25"/>
       <c r="J19" s="15"/>
-    </row>
-    <row r="20" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K19" s="25"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="25"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="82"/>
+      <c r="Q19" s="94"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
+    </row>
+    <row r="20" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
         <v>4</v>
       </c>
@@ -1136,11 +1501,20 @@
       <c r="E20" s="18"/>
       <c r="F20" s="20"/>
       <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
+      <c r="H20" s="20"/>
       <c r="I20" s="18"/>
       <c r="J20" s="19"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K20" s="18"/>
+      <c r="L20" s="64"/>
+      <c r="M20" s="64"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="64"/>
+      <c r="P20" s="79"/>
+      <c r="Q20" s="91"/>
+      <c r="R20" s="64"/>
+      <c r="S20" s="64"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="26" t="s">
         <v>16</v>
       </c>
@@ -1158,13 +1532,30 @@
       <c r="G21" s="27">
         <v>48000</v>
       </c>
-      <c r="H21" s="28"/>
+      <c r="H21" s="29"/>
       <c r="I21" s="27">
         <v>48000</v>
       </c>
       <c r="J21" s="28"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K21" s="27">
+        <v>48000</v>
+      </c>
+      <c r="L21" s="67"/>
+      <c r="M21" s="67"/>
+      <c r="N21" s="27">
+        <v>48000</v>
+      </c>
+      <c r="O21" s="67"/>
+      <c r="P21" s="83">
+        <v>48000</v>
+      </c>
+      <c r="Q21" s="95"/>
+      <c r="R21" s="67">
+        <v>48000</v>
+      </c>
+      <c r="S21" s="67"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>6</v>
       </c>
@@ -1182,13 +1573,30 @@
       <c r="G22" s="27">
         <v>125000</v>
       </c>
-      <c r="H22" s="28"/>
+      <c r="H22" s="29"/>
       <c r="I22" s="27">
         <v>125000</v>
       </c>
       <c r="J22" s="28"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K22" s="27">
+        <v>125000</v>
+      </c>
+      <c r="L22" s="67"/>
+      <c r="M22" s="67"/>
+      <c r="N22" s="27">
+        <v>125000</v>
+      </c>
+      <c r="O22" s="67"/>
+      <c r="P22" s="83">
+        <v>125000</v>
+      </c>
+      <c r="Q22" s="95"/>
+      <c r="R22" s="67">
+        <v>125000</v>
+      </c>
+      <c r="S22" s="67"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C23" s="25"/>
       <c r="D23" s="15"/>
       <c r="E23" s="25"/>
@@ -1197,8 +1605,16 @@
       <c r="H23" s="15"/>
       <c r="I23" s="25"/>
       <c r="J23" s="15"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K23" s="25"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="25"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="82"/>
+      <c r="Q23" s="94"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="23"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
         <v>21</v>
       </c>
@@ -1208,39 +1624,68 @@
       <c r="E24" s="18"/>
       <c r="F24" s="20"/>
       <c r="G24" s="18"/>
-      <c r="H24" s="19"/>
+      <c r="H24" s="20"/>
       <c r="I24" s="18"/>
       <c r="J24" s="19"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K24" s="18"/>
+      <c r="L24" s="64"/>
+      <c r="M24" s="64"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="64"/>
+      <c r="P24" s="79"/>
+      <c r="Q24" s="91"/>
+      <c r="R24" s="64"/>
+      <c r="S24" s="64"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="21" t="s">
         <v>57</v>
       </c>
       <c r="B25" s="21"/>
-      <c r="C25" s="61">
+      <c r="C25" s="60">
         <f>IF(C8&lt;C7,C8/C7*C6,C6)</f>
-        <v>1559.9999999999998</v>
-      </c>
-      <c r="D25" s="62"/>
-      <c r="E25" s="61">
+        <v>2080</v>
+      </c>
+      <c r="D25" s="61"/>
+      <c r="E25" s="60">
         <f>IF(E8&lt;E7,E8/E7*E6,E6)</f>
         <v>1366.6666666666667</v>
       </c>
-      <c r="F25" s="62"/>
-      <c r="G25" s="61">
+      <c r="F25" s="61"/>
+      <c r="G25" s="60">
         <f>IF(G8&lt;G7,G8/G7*G6,G6)</f>
-        <v>1600</v>
-      </c>
-      <c r="H25" s="62"/>
-      <c r="I25" s="61">
+        <v>2080</v>
+      </c>
+      <c r="H25" s="61"/>
+      <c r="I25" s="60">
         <f>IF(I8&lt;I7,I8/I7*I6,I6)</f>
         <v>1600</v>
       </c>
-      <c r="J25" s="60"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="24"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J25" s="61"/>
+      <c r="K25" s="60">
+        <f>IF(K8&lt;K7,K8/K7*K6,K6)</f>
+        <v>1600</v>
+      </c>
+      <c r="L25" s="68"/>
+      <c r="M25" s="68"/>
+      <c r="N25" s="60">
+        <f>IF(N8&lt;N7,N8/N7*N6,N6)</f>
+        <v>1371.4285714285716</v>
+      </c>
+      <c r="O25" s="73"/>
+      <c r="P25" s="84">
+        <f>IF(P8&lt;P7,P8/P7*P6,P6)</f>
+        <v>1066.6666666666667</v>
+      </c>
+      <c r="Q25" s="96"/>
+      <c r="R25" s="73">
+        <f>IF(R8&lt;R7,R8/R7*R6,R6)</f>
+        <v>1280</v>
+      </c>
+      <c r="S25" s="73"/>
+      <c r="T25" s="24"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="30" t="s">
         <v>7</v>
       </c>
@@ -1256,21 +1701,41 @@
       </c>
       <c r="F26" s="32"/>
       <c r="G26" s="55">
-        <f>IF(((G16/G17)+((G29*(G9-G21))))&lt;=100%,((G16/G17)+((G29*(G9-G21)))),100%)</f>
-        <v>0.94255744255744267</v>
+        <f>IF(G9&lt;=125000,((G16/G17)+((G29*(G9-G21)))),101%)</f>
+        <v>1.01</v>
       </c>
       <c r="H26" s="32"/>
       <c r="I26" s="55">
         <f>IF(((I16/I17)+((I29*(I9-I21))))&lt;=100%,((I16/I17)+((I29*(I9-I21)))),100%)</f>
+        <v>0.94255744255744267</v>
+      </c>
+      <c r="J26" s="32"/>
+      <c r="K26" s="55">
+        <f>IF(((K16/K17)+((K29*(K9-K21))))&lt;=100%,((K16/K17)+((K29*(K9-K21)))),100%)</f>
         <v>1</v>
       </c>
-      <c r="J26" s="32"/>
-      <c r="K26" s="30"/>
-      <c r="L26" s="54" t="s">
+      <c r="L26" s="69"/>
+      <c r="M26" s="69"/>
+      <c r="N26" s="55">
+        <f>IF(((N16/N17)+((N29*(N9-N21))))&lt;=100%,((N16/N17)+((N29*(N9-N21)))),100%)</f>
+        <v>0.11538461538461539</v>
+      </c>
+      <c r="O26" s="74"/>
+      <c r="P26" s="85">
+        <f>IF(((P16/P17)+((P29*(P9-P21))))&lt;=100%,((P16/P17)+((P29*(P9-P21)))),100%)</f>
+        <v>0.11538461538461539</v>
+      </c>
+      <c r="Q26" s="97"/>
+      <c r="R26" s="74">
+        <f>IF(((R16/R17)+((R29*(R9-R21))))&lt;=100%,((R16/R17)+((R29*(R9-R21)))),100%)</f>
+        <v>0.16133866133866134</v>
+      </c>
+      <c r="S26" s="74"/>
+      <c r="T26" s="54" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="34" t="s">
         <v>10</v>
       </c>
@@ -1289,19 +1754,39 @@
       <c r="F27" s="15"/>
       <c r="G27" s="35">
         <f>IF(G$9&lt;=125000,G$26*50%*G$17,0)</f>
-        <v>61.266233766233775</v>
+        <v>0</v>
       </c>
       <c r="H27" s="15"/>
       <c r="I27" s="35">
         <f>IF(I$9&lt;=125000,I$26*50%*I$17,0)</f>
-        <v>0</v>
+        <v>61.266233766233775</v>
       </c>
       <c r="J27" s="15"/>
-      <c r="L27" s="36" t="s">
+      <c r="K27" s="35">
+        <f>IF(K$9&lt;=125000,K$26*50%*K$17,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M27" s="23"/>
+      <c r="N27" s="35">
+        <f>IF(N$9&lt;=125000,N$26*50%*N$17,0)</f>
+        <v>7.5</v>
+      </c>
+      <c r="O27" s="75"/>
+      <c r="P27" s="86">
+        <f>IF(P$9&lt;=125000,P$26*50%*P$17,0)</f>
+        <v>7.5</v>
+      </c>
+      <c r="Q27" s="98"/>
+      <c r="R27" s="75">
+        <f>IF(R$9&lt;=125000,R$26*50%*R$17,0)</f>
+        <v>10.487012987012987</v>
+      </c>
+      <c r="S27" s="75"/>
+      <c r="T27" s="36" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="34" t="s">
         <v>11</v>
       </c>
@@ -1320,21 +1805,39 @@
       <c r="F28" s="15"/>
       <c r="G28" s="35">
         <f>IF(G$9&lt;=125000,G$26*70%*G$17,0)</f>
-        <v>85.77272727272728</v>
+        <v>0</v>
       </c>
       <c r="H28" s="15"/>
       <c r="I28" s="35">
         <f>IF(I$9&lt;=125000,I$26*70%*I$17,0)</f>
-        <v>0</v>
+        <v>85.77272727272728</v>
       </c>
       <c r="J28" s="15"/>
-      <c r="L28" s="36" t="s">
+      <c r="K28" s="35">
+        <f>IF(K$9&lt;=125000,K$26*70%*K$17,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M28" s="23"/>
+      <c r="N28" s="35">
+        <f>IF(N$9&lt;=125000,N$26*70%*N$17,0)</f>
+        <v>10.5</v>
+      </c>
+      <c r="O28" s="75"/>
+      <c r="P28" s="86">
+        <f>IF(P$9&lt;=125000,P$26*70%*P$17,0)</f>
+        <v>10.5</v>
+      </c>
+      <c r="Q28" s="98"/>
+      <c r="R28" s="75">
+        <f>IF(R$9&lt;=125000,R$26*70%*R$17,0)</f>
+        <v>14.681818181818182</v>
+      </c>
+      <c r="S28" s="75"/>
+      <c r="T28" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="N28" s="37"/>
-      <c r="O28" s="37"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="34" t="s">
         <v>9</v>
       </c>
@@ -1351,21 +1854,40 @@
       <c r="F29" s="15"/>
       <c r="G29" s="38">
         <f>((1-(G16/G17))/(G22-G21))</f>
-        <v>1.1488511488511489E-5</v>
-      </c>
-      <c r="H29" s="39"/>
+        <v>1.1769480519480519E-5</v>
+      </c>
+      <c r="H29" s="15"/>
       <c r="I29" s="38">
         <f>((1-(I16/I17))/(I22-I21))</f>
         <v>1.1488511488511489E-5</v>
       </c>
       <c r="J29" s="39"/>
-      <c r="L29" s="22" t="s">
+      <c r="K29" s="38">
+        <f>((1-(K16/K17))/(K22-K21))</f>
+        <v>1.1488511488511489E-5</v>
+      </c>
+      <c r="L29" s="70"/>
+      <c r="M29" s="70"/>
+      <c r="N29" s="38">
+        <f>((1-(N16/N17))/(N22-N21))</f>
+        <v>1.1488511488511489E-5</v>
+      </c>
+      <c r="O29" s="76"/>
+      <c r="P29" s="87">
+        <f>((1-(P16/P17))/(P22-P21))</f>
+        <v>1.1488511488511489E-5</v>
+      </c>
+      <c r="Q29" s="99"/>
+      <c r="R29" s="76">
+        <f>((1-(R16/R17))/(R22-R21))</f>
+        <v>1.1488511488511489E-5</v>
+      </c>
+      <c r="S29" s="76"/>
+      <c r="T29" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="N29" s="37"/>
-      <c r="O29" s="37"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="34" t="s">
         <v>53</v>
       </c>
@@ -1379,25 +1901,40 @@
       </c>
       <c r="F30" s="15"/>
       <c r="G30" s="35">
-        <v>10</v>
-      </c>
-      <c r="H30" s="39"/>
+        <v>12.6</v>
+      </c>
+      <c r="H30" s="15"/>
       <c r="I30" s="35">
         <v>10</v>
       </c>
       <c r="J30" s="39"/>
-      <c r="L30" s="22"/>
-      <c r="N30" s="37"/>
-      <c r="O30" s="37"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K30" s="35">
+        <v>10</v>
+      </c>
+      <c r="L30" s="70"/>
+      <c r="M30" s="70"/>
+      <c r="N30" s="35">
+        <v>10</v>
+      </c>
+      <c r="O30" s="75"/>
+      <c r="P30" s="86">
+        <v>11</v>
+      </c>
+      <c r="Q30" s="98"/>
+      <c r="R30" s="75">
+        <v>11</v>
+      </c>
+      <c r="S30" s="75"/>
+      <c r="T30" s="22"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="34" t="s">
         <v>31</v>
       </c>
       <c r="B31" s="34"/>
       <c r="C31" s="31">
         <f>MIN(C7:C8)</f>
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="31">
@@ -1407,26 +1944,45 @@
       <c r="F31" s="15"/>
       <c r="G31" s="31">
         <f>MIN(G7:G8)</f>
-        <v>0.6</v>
-      </c>
-      <c r="H31" s="39"/>
+        <v>0.8</v>
+      </c>
+      <c r="H31" s="15"/>
       <c r="I31" s="31">
         <f>MIN(I7:I8)</f>
         <v>0.6</v>
       </c>
       <c r="J31" s="39"/>
-      <c r="L31" s="22"/>
-      <c r="N31" s="37"/>
-      <c r="O31" s="37"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K31" s="31">
+        <f>MIN(K7:K8)</f>
+        <v>0.6</v>
+      </c>
+      <c r="L31" s="70"/>
+      <c r="M31" s="70"/>
+      <c r="N31" s="31">
+        <f>MIN(N7:N8)</f>
+        <v>0.6</v>
+      </c>
+      <c r="O31" s="77"/>
+      <c r="P31" s="88">
+        <f>MIN(P7:P8)</f>
+        <v>0.4</v>
+      </c>
+      <c r="Q31" s="100"/>
+      <c r="R31" s="77">
+        <f>MIN(R7:R8)</f>
+        <v>0.4</v>
+      </c>
+      <c r="S31" s="77"/>
+      <c r="T31" s="22"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="34" t="s">
         <v>14</v>
       </c>
       <c r="B32" s="34"/>
       <c r="C32" s="25">
         <f>C31*5</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D32" s="15"/>
       <c r="E32" s="25">
@@ -1436,7 +1992,7 @@
       <c r="F32" s="15"/>
       <c r="G32" s="25">
         <f>G31*5</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H32" s="15"/>
       <c r="I32" s="25">
@@ -1444,11 +2000,29 @@
         <v>3</v>
       </c>
       <c r="J32" s="15"/>
-      <c r="L32" s="22"/>
-      <c r="N32" s="37"/>
-      <c r="O32" s="37"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K32" s="25">
+        <f>K31*5</f>
+        <v>3</v>
+      </c>
+      <c r="M32" s="23"/>
+      <c r="N32" s="25">
+        <f>N31*5</f>
+        <v>3</v>
+      </c>
+      <c r="O32" s="23"/>
+      <c r="P32" s="82">
+        <f t="shared" ref="P32" si="0">P31*5</f>
+        <v>2</v>
+      </c>
+      <c r="Q32" s="94"/>
+      <c r="R32" s="23">
+        <f t="shared" ref="R32" si="1">R31*5</f>
+        <v>2</v>
+      </c>
+      <c r="S32" s="23"/>
+      <c r="T32" s="22"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>12</v>
       </c>
@@ -1468,17 +2042,31 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="J33" s="15"/>
-      <c r="L33" s="22"/>
-      <c r="N33" s="37"/>
-      <c r="O33" s="37"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K33" s="25">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="M33" s="23"/>
+      <c r="N33" s="25">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="O33" s="23"/>
+      <c r="P33" s="82">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="Q33" s="94"/>
+      <c r="R33" s="23">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="S33" s="23"/>
+      <c r="T33" s="22"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C34" s="25">
         <f>C32*C33</f>
-        <v>12.299999999999999</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="25">
@@ -1488,7 +2076,7 @@
       <c r="F34" s="15"/>
       <c r="G34" s="25">
         <f>G32*G33</f>
-        <v>12.299999999999999</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="H34" s="15"/>
       <c r="I34" s="25">
@@ -1496,10 +2084,28 @@
         <v>12.299999999999999</v>
       </c>
       <c r="J34" s="15"/>
-      <c r="N34" s="37"/>
-      <c r="O34" s="37"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K34" s="25">
+        <f>K32*K33</f>
+        <v>12.299999999999999</v>
+      </c>
+      <c r="M34" s="23"/>
+      <c r="N34" s="25">
+        <f>N32*N33</f>
+        <v>12.299999999999999</v>
+      </c>
+      <c r="O34" s="23"/>
+      <c r="P34" s="82">
+        <f>P32*P33</f>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="Q34" s="94"/>
+      <c r="R34" s="23">
+        <f>R32*R33</f>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="S34" s="23"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="34"/>
       <c r="B35" s="34"/>
       <c r="C35" s="38"/>
@@ -1507,14 +2113,21 @@
       <c r="E35" s="38"/>
       <c r="F35" s="15"/>
       <c r="G35" s="38"/>
-      <c r="H35" s="39"/>
+      <c r="H35" s="15"/>
       <c r="I35" s="38"/>
       <c r="J35" s="39"/>
-      <c r="L35" s="22"/>
-      <c r="N35" s="37"/>
-      <c r="O35" s="37"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K35" s="38"/>
+      <c r="L35" s="70"/>
+      <c r="M35" s="70"/>
+      <c r="N35" s="38"/>
+      <c r="O35" s="76"/>
+      <c r="P35" s="87"/>
+      <c r="Q35" s="99"/>
+      <c r="R35" s="76"/>
+      <c r="S35" s="76"/>
+      <c r="T35" s="22"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" s="16" t="s">
         <v>47</v>
       </c>
@@ -1524,13 +2137,20 @@
       <c r="E36" s="18"/>
       <c r="F36" s="20"/>
       <c r="G36" s="18"/>
-      <c r="H36" s="19"/>
+      <c r="H36" s="20"/>
       <c r="I36" s="18"/>
       <c r="J36" s="19"/>
-      <c r="M36" s="37"/>
-      <c r="N36" s="37"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K36" s="18"/>
+      <c r="L36" s="64"/>
+      <c r="M36" s="64"/>
+      <c r="N36" s="18"/>
+      <c r="O36" s="64"/>
+      <c r="P36" s="79"/>
+      <c r="Q36" s="91"/>
+      <c r="R36" s="64"/>
+      <c r="S36" s="64"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="34" t="s">
         <v>23</v>
       </c>
@@ -1548,18 +2168,38 @@
       </c>
       <c r="F37" s="41"/>
       <c r="G37" s="40">
-        <f>IF((G17*(1-G26))&gt;G30,(G17*(1-G26)),IF(G9&lt;=125000,G30,0))</f>
-        <v>10</v>
+        <f>IF((G17*(1-G26))&gt;G30,(G17*(1-G26)),IF(G26&lt;=100%,G30,IF(G26&gt;100%,0)))</f>
+        <v>0</v>
       </c>
       <c r="H37" s="41"/>
       <c r="I37" s="40">
         <f>IF((I17*(1-I26))&gt;I30,(I17*(1-I26)),IF(I9&lt;=125000,I30,0))</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J37" s="41"/>
-      <c r="K37" s="42"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K37" s="40">
+        <f>IF((K17*(1-K26))&gt;K30,(K17*(1-K26)),IF(K9&lt;=125000,K30,0))</f>
+        <v>0</v>
+      </c>
+      <c r="L37" s="71"/>
+      <c r="M37" s="71"/>
+      <c r="N37" s="40">
+        <f>IF((N17*(1-N26))&gt;N30,(N17*(1-N26)),IF(N9&lt;=125000,N30,0))</f>
+        <v>115</v>
+      </c>
+      <c r="O37" s="71"/>
+      <c r="P37" s="89">
+        <f>IF((P17*(1-P26))&gt;P30,(P17*(1-P26)),IF(P9&lt;=125000,P30,0))</f>
+        <v>115</v>
+      </c>
+      <c r="Q37" s="101"/>
+      <c r="R37" s="71">
+        <f>IF((R17*(1-R26))&gt;R30,(R17*(1-R26)),IF(R9&lt;=125000,R30,0))</f>
+        <v>109.02597402597402</v>
+      </c>
+      <c r="S37" s="71"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="34" t="str">
         <f>A12</f>
         <v>Geschwisternbonus 2. Kind</v>
@@ -1569,12 +2209,12 @@
       </c>
       <c r="C38" s="40">
         <f>IF(C12,C27,0)</f>
-        <v>9.3831168831168839</v>
+        <v>0</v>
       </c>
       <c r="D38" s="41"/>
       <c r="E38" s="40">
         <f>IF(E12,E27,0)</f>
-        <v>37.629870129870127</v>
+        <v>0</v>
       </c>
       <c r="F38" s="41"/>
       <c r="G38" s="40">
@@ -1587,10 +2227,30 @@
         <v>0</v>
       </c>
       <c r="J38" s="41"/>
-      <c r="K38" s="42"/>
-      <c r="L38" s="56"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K38" s="40">
+        <f>IF(K12,K27,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L38" s="71"/>
+      <c r="M38" s="71"/>
+      <c r="N38" s="40">
+        <f>IF(N12,N27,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O38" s="71"/>
+      <c r="P38" s="89">
+        <f>IF(P12,P27,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q38" s="101"/>
+      <c r="R38" s="71">
+        <f>IF(R12,R27,0)</f>
+        <v>0</v>
+      </c>
+      <c r="S38" s="71"/>
+      <c r="T38" s="56"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="34" t="str">
         <f>A13</f>
         <v>Geschwisternbonus 3. Kind</v>
@@ -1618,10 +2278,30 @@
         <v>0</v>
       </c>
       <c r="J39" s="41"/>
-      <c r="K39" s="42"/>
-      <c r="L39" s="22"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K39" s="40">
+        <f>IF(K13,K28,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L39" s="71"/>
+      <c r="M39" s="71"/>
+      <c r="N39" s="40">
+        <f>IF(N13,N28,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O39" s="71"/>
+      <c r="P39" s="89">
+        <f>IF(P13,P28,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q39" s="101"/>
+      <c r="R39" s="71">
+        <f>IF(R13,R28,0)</f>
+        <v>0</v>
+      </c>
+      <c r="S39" s="71"/>
+      <c r="T39" s="22"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" s="43" t="s">
         <v>42</v>
       </c>
@@ -1630,27 +2310,47 @@
       </c>
       <c r="C40" s="40">
         <f>C39+C38+C37</f>
-        <v>150.61688311688312</v>
+        <v>141.23376623376623</v>
       </c>
       <c r="D40" s="41"/>
       <c r="E40" s="40">
         <f>E39+E38+E37</f>
-        <v>122.37012987012987</v>
+        <v>84.740259740259745</v>
       </c>
       <c r="F40" s="41"/>
       <c r="G40" s="40">
         <f>G39+G38+G37</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H40" s="41"/>
       <c r="I40" s="40">
         <f>I39+I38+I37</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J40" s="41"/>
-      <c r="K40" s="42"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K40" s="40">
+        <f>K39+K38+K37</f>
+        <v>0</v>
+      </c>
+      <c r="L40" s="71"/>
+      <c r="M40" s="71"/>
+      <c r="N40" s="40">
+        <f>N39+N38+N37</f>
+        <v>115</v>
+      </c>
+      <c r="O40" s="71"/>
+      <c r="P40" s="89">
+        <f>P39+P38+P37</f>
+        <v>115</v>
+      </c>
+      <c r="Q40" s="101"/>
+      <c r="R40" s="71">
+        <f>R39+R38+R37</f>
+        <v>109.02597402597402</v>
+      </c>
+      <c r="S40" s="71"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" s="44" t="s">
         <v>41</v>
       </c>
@@ -1659,27 +2359,47 @@
       </c>
       <c r="C41" s="40">
         <f>C40*C34</f>
-        <v>1852.5876623376621</v>
+        <v>2316.2337662337659</v>
       </c>
       <c r="D41" s="41"/>
       <c r="E41" s="40">
         <f>E40*E34</f>
-        <v>1254.2938311688313</v>
+        <v>868.58766233766244</v>
       </c>
       <c r="F41" s="41"/>
       <c r="G41" s="40">
         <f>G40*G34</f>
-        <v>122.99999999999999</v>
+        <v>0</v>
       </c>
       <c r="H41" s="41"/>
       <c r="I41" s="40">
         <f>I40*I34</f>
-        <v>0</v>
+        <v>122.99999999999999</v>
       </c>
       <c r="J41" s="41"/>
-      <c r="K41" s="42"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K41" s="40">
+        <f>K40*K34</f>
+        <v>0</v>
+      </c>
+      <c r="L41" s="71"/>
+      <c r="M41" s="71"/>
+      <c r="N41" s="40">
+        <f>N40*N34</f>
+        <v>1414.4999999999998</v>
+      </c>
+      <c r="O41" s="71"/>
+      <c r="P41" s="89">
+        <f>P40*P34</f>
+        <v>942.99999999999989</v>
+      </c>
+      <c r="Q41" s="101"/>
+      <c r="R41" s="71">
+        <f>R40*R34</f>
+        <v>894.01298701298686</v>
+      </c>
+      <c r="S41" s="71"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" s="34" t="s">
         <v>33</v>
       </c>
@@ -1688,27 +2408,47 @@
       </c>
       <c r="C42" s="40">
         <f>C25-C41</f>
-        <v>-292.58766233766232</v>
+        <v>-236.23376623376589</v>
       </c>
       <c r="D42" s="41"/>
       <c r="E42" s="40">
         <f>E25-E41</f>
-        <v>112.37283549783547</v>
+        <v>498.07900432900431</v>
       </c>
       <c r="F42" s="41"/>
       <c r="G42" s="40">
         <f>G25-G41</f>
-        <v>1477</v>
+        <v>2080</v>
       </c>
       <c r="H42" s="41"/>
       <c r="I42" s="40">
         <f>I25-I41</f>
+        <v>1477</v>
+      </c>
+      <c r="J42" s="41"/>
+      <c r="K42" s="40">
+        <f>K25-K41</f>
         <v>1600</v>
       </c>
-      <c r="J42" s="41"/>
-      <c r="K42" s="42"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L42" s="71"/>
+      <c r="M42" s="71"/>
+      <c r="N42" s="40">
+        <f>N25-N41</f>
+        <v>-43.071428571428214</v>
+      </c>
+      <c r="O42" s="71"/>
+      <c r="P42" s="89">
+        <f>P25-P41</f>
+        <v>123.66666666666686</v>
+      </c>
+      <c r="Q42" s="101"/>
+      <c r="R42" s="71">
+        <f>R25-R41</f>
+        <v>385.98701298701314</v>
+      </c>
+      <c r="S42" s="71"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="34" t="s">
         <v>36</v>
       </c>
@@ -1717,7 +2457,7 @@
       </c>
       <c r="C43" s="40">
         <f>C16*C34</f>
-        <v>184.49999999999997</v>
+        <v>245.99999999999997</v>
       </c>
       <c r="D43" s="41"/>
       <c r="E43" s="40">
@@ -1727,7 +2467,7 @@
       <c r="F43" s="41"/>
       <c r="G43" s="40">
         <f>G16*G34</f>
-        <v>184.49999999999997</v>
+        <v>245.99999999999997</v>
       </c>
       <c r="H43" s="41"/>
       <c r="I43" s="40">
@@ -1735,12 +2475,32 @@
         <v>184.49999999999997</v>
       </c>
       <c r="J43" s="41"/>
-      <c r="K43" s="42"/>
-      <c r="L43" s="53" t="s">
+      <c r="K43" s="40">
+        <f>K16*K34</f>
+        <v>184.49999999999997</v>
+      </c>
+      <c r="L43" s="71"/>
+      <c r="M43" s="71"/>
+      <c r="N43" s="40">
+        <f>N16*N34</f>
+        <v>184.49999999999997</v>
+      </c>
+      <c r="O43" s="71"/>
+      <c r="P43" s="89">
+        <f>P16*P34</f>
+        <v>122.99999999999999</v>
+      </c>
+      <c r="Q43" s="101"/>
+      <c r="R43" s="71">
+        <f>R16*R34</f>
+        <v>122.99999999999999</v>
+      </c>
+      <c r="S43" s="71"/>
+      <c r="T43" s="53" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" s="34" t="s">
         <v>40</v>
       </c>
@@ -1749,12 +2509,12 @@
       </c>
       <c r="C44" s="40">
         <f>IF((C43-C42)&gt;=0,(C43-C42),0)</f>
-        <v>477.08766233766232</v>
+        <v>482.23376623376589</v>
       </c>
       <c r="D44" s="41"/>
       <c r="E44" s="40">
         <f>IF((E43-E42)&gt;=0,(E43-E42),0)</f>
-        <v>41.377164502164533</v>
+        <v>0</v>
       </c>
       <c r="F44" s="41"/>
       <c r="G44" s="40">
@@ -1767,9 +2527,29 @@
         <v>0</v>
       </c>
       <c r="J44" s="41"/>
-      <c r="K44" s="42"/>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K44" s="40">
+        <f>IF((K43-K42)&gt;=0,(K43-K42),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L44" s="71"/>
+      <c r="M44" s="71"/>
+      <c r="N44" s="40">
+        <f>IF((N43-N42)&gt;=0,(N43-N42),0)</f>
+        <v>227.57142857142819</v>
+      </c>
+      <c r="O44" s="71"/>
+      <c r="P44" s="89">
+        <f>IF((P43-P42)&gt;=0,(P43-P42),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q44" s="101"/>
+      <c r="R44" s="71">
+        <f>IF((R43-R42)&gt;=0,(R43-R42),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S44" s="71"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" s="44" t="s">
         <v>43</v>
       </c>
@@ -1778,27 +2558,47 @@
       </c>
       <c r="C45" s="40">
         <f>C41-C44</f>
-        <v>1375.4999999999998</v>
+        <v>1834</v>
       </c>
       <c r="D45" s="41"/>
       <c r="E45" s="40">
         <f>E41-E44</f>
-        <v>1212.9166666666667</v>
+        <v>868.58766233766244</v>
       </c>
       <c r="F45" s="41"/>
       <c r="G45" s="40">
         <f>G41-G44</f>
-        <v>122.99999999999999</v>
+        <v>0</v>
       </c>
       <c r="H45" s="41"/>
       <c r="I45" s="40">
         <f>I41-I44</f>
-        <v>0</v>
+        <v>122.99999999999999</v>
       </c>
       <c r="J45" s="41"/>
-      <c r="K45" s="42"/>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K45" s="40">
+        <f>K41-K44</f>
+        <v>0</v>
+      </c>
+      <c r="L45" s="71"/>
+      <c r="M45" s="71"/>
+      <c r="N45" s="40">
+        <f>N41-N44</f>
+        <v>1186.9285714285716</v>
+      </c>
+      <c r="O45" s="71"/>
+      <c r="P45" s="89">
+        <f>P41-P44</f>
+        <v>942.99999999999989</v>
+      </c>
+      <c r="Q45" s="101"/>
+      <c r="R45" s="71">
+        <f>R41-R44</f>
+        <v>894.01298701298686</v>
+      </c>
+      <c r="S45" s="71"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" s="34" t="s">
         <v>28</v>
       </c>
@@ -1825,9 +2625,29 @@
         <v>0</v>
       </c>
       <c r="J46" s="41"/>
-      <c r="K46" s="42"/>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K46" s="40">
+        <f>K10</f>
+        <v>0</v>
+      </c>
+      <c r="L46" s="71"/>
+      <c r="M46" s="71"/>
+      <c r="N46" s="40">
+        <f>N10</f>
+        <v>0</v>
+      </c>
+      <c r="O46" s="71"/>
+      <c r="P46" s="89">
+        <f>P10</f>
+        <v>0</v>
+      </c>
+      <c r="Q46" s="101"/>
+      <c r="R46" s="71">
+        <f>R10</f>
+        <v>10</v>
+      </c>
+      <c r="S46" s="71"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" s="21" t="s">
         <v>29</v>
       </c>
@@ -1854,9 +2674,29 @@
         <v>0</v>
       </c>
       <c r="J47" s="41"/>
-      <c r="K47" s="42"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K47" s="40">
+        <f>IF(K11,K18,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L47" s="71"/>
+      <c r="M47" s="71"/>
+      <c r="N47" s="40">
+        <f>IF(N11,N18,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O47" s="71"/>
+      <c r="P47" s="89">
+        <f>IF(P11,P18,0)</f>
+        <v>32</v>
+      </c>
+      <c r="Q47" s="101"/>
+      <c r="R47" s="71">
+        <f>IF(R11,R18,0)</f>
+        <v>0</v>
+      </c>
+      <c r="S47" s="71"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" s="34" t="s">
         <v>37</v>
       </c>
@@ -1883,8 +2723,29 @@
         <v>0</v>
       </c>
       <c r="J48" s="41"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K48" s="40">
+        <f>(K46+K47)*K34</f>
+        <v>0</v>
+      </c>
+      <c r="L48" s="71"/>
+      <c r="M48" s="71"/>
+      <c r="N48" s="40">
+        <f>(N46+N47)*N34</f>
+        <v>0</v>
+      </c>
+      <c r="O48" s="71"/>
+      <c r="P48" s="89">
+        <f>(P46+P47)*P34</f>
+        <v>262.39999999999998</v>
+      </c>
+      <c r="Q48" s="101"/>
+      <c r="R48" s="71">
+        <f>(R46+R47)*R34</f>
+        <v>82</v>
+      </c>
+      <c r="S48" s="71"/>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" s="45" t="s">
         <v>44</v>
       </c>
@@ -1893,36 +2754,57 @@
       </c>
       <c r="C49" s="46">
         <f>C45+C48</f>
-        <v>1375.4999999999998</v>
+        <v>1834</v>
       </c>
       <c r="D49" s="47"/>
       <c r="E49" s="46">
         <f>E45+E48</f>
-        <v>1540.9166666666667</v>
+        <v>1196.5876623376626</v>
       </c>
       <c r="F49" s="47"/>
       <c r="G49" s="46">
         <f>G45+G48</f>
-        <v>122.99999999999999</v>
+        <v>0</v>
       </c>
       <c r="H49" s="47"/>
       <c r="I49" s="46">
         <f>I45+I48</f>
-        <v>0</v>
+        <v>122.99999999999999</v>
       </c>
       <c r="J49" s="47"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K49" s="46">
+        <f>K45+K48</f>
+        <v>0</v>
+      </c>
+      <c r="L49" s="72"/>
+      <c r="M49" s="72"/>
+      <c r="N49" s="46">
+        <f>N45+N48</f>
+        <v>1186.9285714285716</v>
+      </c>
+      <c r="O49" s="46"/>
+      <c r="P49" s="46">
+        <f>P45+P48</f>
+        <v>1205.3999999999999</v>
+      </c>
+      <c r="Q49" s="102"/>
+      <c r="R49" s="72">
+        <f>R45+R48</f>
+        <v>976.01298701298686</v>
+      </c>
+      <c r="S49" s="46"/>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
         <v>56</v>
       </c>
       <c r="C50" s="58">
         <f>IF((C34*(C38+C39))&lt;C49,(C34*(C38+C39)),(C49-(C37*C34)))</f>
-        <v>115.41233766233766</v>
+        <v>0</v>
       </c>
       <c r="E50" s="58">
         <f>IF((E34*(E38+E39))&lt;E49,(E34*(E38+E39)),(E49-(E37*E34)))</f>
-        <v>385.70616883116878</v>
+        <v>0</v>
       </c>
       <c r="G50" s="58">
         <f>IF((G34*(G38+G39))&lt;G49,(G34*(G38+G39)),(G49-(G37*G34)))</f>
@@ -1932,16 +2814,213 @@
         <f>IF((I34*(I38+I39))&lt;I49,(I34*(I38+I39)),(I49-(I37*I34)))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K50" s="58">
+        <f>IF((K34*(K38+K39))&lt;K49,(K34*(K38+K39)),(K49-(K37*K34)))</f>
+        <v>0</v>
+      </c>
+      <c r="N50" s="58">
+        <f>IF((N34*(N38+N39))&lt;N49,(N34*(N38+N39)),(N49-(N37*N34)))</f>
+        <v>0</v>
+      </c>
+      <c r="O50" s="58"/>
+      <c r="P50" s="103">
+        <f>IF((P34*(P38+P39))&lt;P49,(P34*(P38+P39)),(P49-(P37*P34)))</f>
+        <v>0</v>
+      </c>
+      <c r="Q50" s="104"/>
+      <c r="R50" s="58">
+        <f>IF((R34*(R38+R39))&lt;R49,(R34*(R38+R39)),(R49-(R37*R34)))</f>
+        <v>0</v>
+      </c>
+      <c r="S50" s="58"/>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="P51" s="105"/>
+      <c r="Q51" s="94"/>
+      <c r="R51"/>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C52" s="59"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C53" s="59"/>
-      <c r="E53" s="59"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L56" s="48"/>
+      <c r="P52" s="105"/>
+      <c r="Q52" s="94"/>
+      <c r="R52"/>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53"/>
+      <c r="C53" s="62">
+        <f>SUM(C48,C41)</f>
+        <v>2316.2337662337659</v>
+      </c>
+      <c r="D53" s="62"/>
+      <c r="E53" s="62">
+        <f t="shared" ref="E53:K53" si="2">SUM(E48,E41)</f>
+        <v>1196.5876623376626</v>
+      </c>
+      <c r="F53" s="62"/>
+      <c r="G53" s="62">
+        <f t="shared" ref="G53" si="3">SUM(G48,G41)</f>
+        <v>0</v>
+      </c>
+      <c r="H53" s="62"/>
+      <c r="I53" s="62">
+        <f t="shared" si="2"/>
+        <v>122.99999999999999</v>
+      </c>
+      <c r="J53" s="62"/>
+      <c r="K53" s="62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N53" s="62">
+        <f t="shared" ref="N53" si="4">SUM(N48,N41)</f>
+        <v>1414.4999999999998</v>
+      </c>
+      <c r="O53" s="62"/>
+      <c r="P53" s="106">
+        <f>SUM(P48,P41)</f>
+        <v>1205.3999999999999</v>
+      </c>
+      <c r="Q53" s="94"/>
+      <c r="R53" s="62">
+        <f>SUM(R48,R41)</f>
+        <v>976.01298701298686</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54"/>
+      <c r="C54" s="62">
+        <f>IF(C42&lt;0,C41+C42,C41)+C48</f>
+        <v>2080</v>
+      </c>
+      <c r="D54" s="62"/>
+      <c r="E54" s="62">
+        <f t="shared" ref="E54:K54" si="5">IF(E42&lt;0,E41+E42,E41)+E48</f>
+        <v>1196.5876623376626</v>
+      </c>
+      <c r="F54" s="62"/>
+      <c r="G54" s="62">
+        <f t="shared" ref="G54" si="6">IF(G42&lt;0,G41+G42,G41)+G48</f>
+        <v>0</v>
+      </c>
+      <c r="H54" s="62"/>
+      <c r="I54" s="62">
+        <f t="shared" si="5"/>
+        <v>122.99999999999999</v>
+      </c>
+      <c r="J54" s="62"/>
+      <c r="K54" s="62">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N54" s="62">
+        <f t="shared" ref="N54" si="7">IF(N42&lt;0,N41+N42,N41)+N48</f>
+        <v>1371.4285714285716</v>
+      </c>
+      <c r="O54" s="62"/>
+      <c r="P54" s="106">
+        <f>IF(P42&lt;0,P41+P42,P41)+P48</f>
+        <v>1205.3999999999999</v>
+      </c>
+      <c r="Q54" s="94"/>
+      <c r="R54" s="62">
+        <f>IF(R42&lt;0,R41+R42,R41)+R48</f>
+        <v>976.01298701298686</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55"/>
+      <c r="C55" s="62">
+        <f>IF(C43&gt;C44,C44,C43)</f>
+        <v>245.99999999999997</v>
+      </c>
+      <c r="D55" s="62"/>
+      <c r="E55" s="62">
+        <f t="shared" ref="E55:K55" si="8">IF(E43&gt;E44,E44,E43)</f>
+        <v>0</v>
+      </c>
+      <c r="F55" s="62"/>
+      <c r="G55" s="62">
+        <f t="shared" ref="G55" si="9">IF(G43&gt;G44,G44,G43)</f>
+        <v>0</v>
+      </c>
+      <c r="H55" s="62"/>
+      <c r="I55" s="62">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J55" s="62"/>
+      <c r="K55" s="62">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="N55" s="62">
+        <f t="shared" ref="N55" si="10">IF(N43&gt;N44,N44,N43)</f>
+        <v>184.49999999999997</v>
+      </c>
+      <c r="O55" s="62"/>
+      <c r="P55" s="106">
+        <f>IF(P43&gt;P44,P44,P43)</f>
+        <v>0</v>
+      </c>
+      <c r="Q55" s="94"/>
+      <c r="R55" s="62">
+        <f>IF(R43&gt;R44,R44,R43)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56"/>
+      <c r="C56" s="62">
+        <f>C54-C55</f>
+        <v>1834</v>
+      </c>
+      <c r="D56" s="62"/>
+      <c r="E56" s="62">
+        <f t="shared" ref="E56:K56" si="11">E54-E55</f>
+        <v>1196.5876623376626</v>
+      </c>
+      <c r="F56" s="62"/>
+      <c r="G56" s="62">
+        <f t="shared" ref="G56" si="12">G54-G55</f>
+        <v>0</v>
+      </c>
+      <c r="H56" s="62"/>
+      <c r="I56" s="62">
+        <f t="shared" si="11"/>
+        <v>122.99999999999999</v>
+      </c>
+      <c r="J56" s="62"/>
+      <c r="K56" s="62">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N56" s="62">
+        <f t="shared" ref="N56" si="13">N54-N55</f>
+        <v>1186.9285714285716</v>
+      </c>
+      <c r="O56" s="62"/>
+      <c r="P56" s="106">
+        <f t="shared" ref="P56" si="14">P54-P55</f>
+        <v>1205.3999999999999</v>
+      </c>
+      <c r="Q56" s="94"/>
+      <c r="R56" s="62">
+        <f t="shared" ref="R56" si="15">R54-R55</f>
+        <v>976.01298701298686</v>
+      </c>
+      <c r="T56" s="48"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
@@ -1958,37 +3037,37 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="52.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="1.5546875" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.5546875" customWidth="1"/>
-    <col min="7" max="7" width="3.44140625" customWidth="1"/>
-    <col min="8" max="8" width="103.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.33203125" customWidth="1"/>
+    <col min="1" max="1" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="1.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.5703125" customWidth="1"/>
+    <col min="7" max="7" width="3.42578125" customWidth="1"/>
+    <col min="8" max="8" width="103.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.28515625" customWidth="1"/>
     <col min="15" max="15" width="47" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="13" t="s">
@@ -2002,7 +3081,7 @@
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>46</v>
       </c>
@@ -2014,7 +3093,7 @@
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
         <v>45</v>
       </c>
@@ -2032,7 +3111,7 @@
       <c r="G6" s="11"/>
       <c r="H6" s="22"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
         <v>13</v>
       </c>
@@ -2048,7 +3127,7 @@
       <c r="G7" s="23"/>
       <c r="H7" s="24"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
         <v>30</v>
       </c>
@@ -2064,7 +3143,7 @@
       <c r="G8" s="23"/>
       <c r="H8" s="24"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
         <v>8</v>
       </c>
@@ -2082,7 +3161,7 @@
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
         <v>22</v>
       </c>
@@ -2100,7 +3179,7 @@
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
         <v>26</v>
       </c>
@@ -2118,7 +3197,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
         <v>27</v>
       </c>
@@ -2136,7 +3215,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="13"/>
@@ -2146,7 +3225,7 @@
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>5</v>
       </c>
@@ -2158,7 +3237,7 @@
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>0</v>
       </c>
@@ -2176,7 +3255,7 @@
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
     </row>
-    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>3</v>
       </c>
@@ -2194,7 +3273,7 @@
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="37" t="s">
         <v>15</v>
       </c>
@@ -2211,7 +3290,7 @@
       <c r="F17" s="52"/>
       <c r="G17" s="11"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="25"/>
@@ -2221,7 +3300,7 @@
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
         <v>4</v>
       </c>
@@ -2233,7 +3312,7 @@
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="26" t="s">
         <v>16</v>
       </c>
@@ -2251,7 +3330,7 @@
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>6</v>
       </c>
@@ -2269,7 +3348,7 @@
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="25"/>
@@ -2279,7 +3358,7 @@
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
         <v>21</v>
       </c>
@@ -2291,7 +3370,7 @@
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="30" t="s">
         <v>7</v>
       </c>
@@ -2311,7 +3390,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="34" t="s">
         <v>10</v>
       </c>
@@ -2333,7 +3412,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="34" t="s">
         <v>11</v>
       </c>
@@ -2355,7 +3434,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="34" t="s">
         <v>9</v>
       </c>
@@ -2375,7 +3454,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="34" t="s">
         <v>52</v>
       </c>
@@ -2391,7 +3470,7 @@
       <c r="G28" s="11"/>
       <c r="H28" s="22"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="34" t="s">
         <v>31</v>
       </c>
@@ -2409,7 +3488,7 @@
       <c r="G29" s="11"/>
       <c r="H29" s="22"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="34" t="s">
         <v>14</v>
       </c>
@@ -2427,7 +3506,7 @@
       <c r="G30" s="11"/>
       <c r="H30" s="22"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>12</v>
       </c>
@@ -2443,7 +3522,7 @@
       <c r="G31" s="11"/>
       <c r="H31" s="22"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>32</v>
       </c>
@@ -2461,7 +3540,7 @@
       <c r="G32" s="11"/>
       <c r="H32" s="22"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="34"/>
       <c r="B33" s="34"/>
       <c r="C33" s="38"/>
@@ -2471,7 +3550,7 @@
       <c r="G33" s="11"/>
       <c r="H33" s="22"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
         <v>47</v>
       </c>
@@ -2482,7 +3561,7 @@
       <c r="F34" s="20"/>
       <c r="G34" s="11"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="34" t="s">
         <v>23</v>
       </c>
@@ -2501,7 +3580,7 @@
       <c r="F35" s="41"/>
       <c r="G35" s="42"/>
     </row>
-    <row r="36" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="34" t="str">
         <f>A11</f>
         <v>Geschwisternbonus 2. Kind</v>
@@ -2522,7 +3601,7 @@
       <c r="G36" s="42"/>
       <c r="H36" s="11"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="34" t="str">
         <f>A12</f>
         <v>Geschwisternbonus 3. Kind</v>
@@ -2543,7 +3622,7 @@
       <c r="G37" s="42"/>
       <c r="H37" s="11"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="43" t="s">
         <v>42</v>
       </c>
@@ -2563,7 +3642,7 @@
       <c r="G38" s="42"/>
       <c r="H38" s="11"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="44" t="s">
         <v>41</v>
       </c>
@@ -2583,7 +3662,7 @@
       <c r="G39" s="42"/>
       <c r="H39" s="11"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="34" t="s">
         <v>33</v>
       </c>
@@ -2603,7 +3682,7 @@
       <c r="G40" s="42"/>
       <c r="H40" s="11"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="34" t="s">
         <v>36</v>
       </c>
@@ -2625,7 +3704,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="34" t="s">
         <v>40</v>
       </c>
@@ -2645,7 +3724,7 @@
       <c r="G42" s="42"/>
       <c r="H42" s="11"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="44" t="s">
         <v>43</v>
       </c>
@@ -2665,7 +3744,7 @@
       <c r="G43" s="42"/>
       <c r="H43" s="11"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="34" t="s">
         <v>28</v>
       </c>
@@ -2685,7 +3764,7 @@
       <c r="G44" s="42"/>
       <c r="H44" s="11"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="34" t="s">
         <v>37</v>
       </c>
@@ -2705,7 +3784,7 @@
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="45" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
KIBON-2271: BG Calculation aufgrung von Einkommen darf den Maximalwert nicht übersteigen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/test/java/ch/dvbern/ebegu/rechner/BG_Rechner_Luzern_0.1_Stand_Dez21.xlsx
+++ b/ebegu-server/src/test/java/ch/dvbern/ebegu/rechner/BG_Rechner_Luzern_0.1_Stand_Dez21.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ebegu\ebegu-server\src\test\java\ch\dvbern\ebegu\rechner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FF3834-A4B5-45D8-B01B-D6042E2298F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E408001B-241E-46D5-B0D7-710F585DC7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="63">
   <si>
     <t>Minimaltarif</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>Betreuungsgutschein in CHF (VergOhneBeruecksichtigungMinimalbetrag)</t>
+  </si>
+  <si>
+    <t>maximal maximaler Gutschein</t>
   </si>
 </sst>
 </file>
@@ -412,7 +415,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -487,17 +490,12 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="8" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="8" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
@@ -584,6 +582,17 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Eingabe" xfId="2" builtinId="20"/>
@@ -866,16 +875,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T56"/>
+  <dimension ref="A1:X57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T50" sqref="T50"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50" style="11" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" style="11" customWidth="1"/>
     <col min="3" max="3" width="16" style="11" customWidth="1"/>
     <col min="4" max="4" width="3" style="11" customWidth="1"/>
     <col min="5" max="5" width="16" style="11" customWidth="1"/>
@@ -892,41 +901,45 @@
     <col min="16" max="16" width="15.5703125" customWidth="1"/>
     <col min="17" max="17" width="3.5703125" style="11" customWidth="1"/>
     <col min="18" max="18" width="15.5703125" style="11" customWidth="1"/>
-    <col min="19" max="19" width="3.7109375" style="11" customWidth="1"/>
-    <col min="20" max="20" width="94.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="11.42578125" style="11"/>
+    <col min="19" max="19" width="3.85546875" style="11" customWidth="1"/>
+    <col min="20" max="20" width="15.7109375" style="11" customWidth="1"/>
+    <col min="21" max="21" width="3.140625" style="11" customWidth="1"/>
+    <col min="22" max="22" width="94.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" style="11"/>
+    <col min="24" max="24" width="12.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="11.42578125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="49"/>
-    </row>
-    <row r="3" spans="1:20" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B2" s="48"/>
+    </row>
+    <row r="3" spans="1:22" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="C4" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="57">
+      <c r="D4" s="54">
         <v>1</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="57">
+      <c r="F4" s="54">
         <v>2</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="57">
+      <c r="H4" s="54">
         <v>3</v>
       </c>
       <c r="I4" s="13" t="s">
@@ -938,30 +951,36 @@
       <c r="K4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="63">
+      <c r="L4" s="60">
         <v>2</v>
       </c>
-      <c r="M4" s="63"/>
+      <c r="M4" s="60"/>
       <c r="N4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="O4" s="63">
+      <c r="O4" s="60">
         <v>3</v>
       </c>
-      <c r="P4" s="78" t="s">
+      <c r="P4" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="Q4" s="90">
+      <c r="Q4" s="87">
         <v>4</v>
       </c>
-      <c r="R4" s="63" t="s">
+      <c r="R4" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="S4" s="63">
+      <c r="S4" s="87">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T4" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="U4" s="60">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>46</v>
       </c>
@@ -975,16 +994,18 @@
       <c r="I5" s="18"/>
       <c r="J5" s="19"/>
       <c r="K5" s="18"/>
-      <c r="L5" s="64"/>
-      <c r="M5" s="64"/>
+      <c r="L5" s="61"/>
+      <c r="M5" s="61"/>
       <c r="N5" s="18"/>
-      <c r="O5" s="64"/>
-      <c r="P5" s="79"/>
-      <c r="Q5" s="91"/>
-      <c r="R5" s="64"/>
-      <c r="S5" s="64"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="O5" s="61"/>
+      <c r="P5" s="76"/>
+      <c r="Q5" s="88"/>
+      <c r="R5" s="61"/>
+      <c r="S5" s="88"/>
+      <c r="T5" s="61"/>
+      <c r="U5" s="61"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
         <v>45</v>
       </c>
@@ -1010,23 +1031,27 @@
       <c r="K6" s="4">
         <v>1600</v>
       </c>
-      <c r="L6" s="65"/>
-      <c r="M6" s="65"/>
+      <c r="L6" s="62"/>
+      <c r="M6" s="62"/>
       <c r="N6" s="4">
         <v>1600</v>
       </c>
-      <c r="O6" s="65"/>
-      <c r="P6" s="80">
+      <c r="O6" s="62"/>
+      <c r="P6" s="77">
         <v>1600</v>
       </c>
-      <c r="Q6" s="92"/>
-      <c r="R6" s="65">
+      <c r="Q6" s="89"/>
+      <c r="R6" s="62">
         <v>1600</v>
       </c>
-      <c r="S6" s="65"/>
-      <c r="T6" s="22"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S6" s="89"/>
+      <c r="T6" s="62">
+        <v>1600</v>
+      </c>
+      <c r="U6" s="62"/>
+      <c r="V6" s="107"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
         <v>13</v>
       </c>
@@ -1050,23 +1075,27 @@
       <c r="K7" s="6">
         <v>0.6</v>
       </c>
-      <c r="L7" s="66"/>
-      <c r="M7" s="66"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="63"/>
       <c r="N7" s="6">
         <v>0.7</v>
       </c>
-      <c r="O7" s="66"/>
-      <c r="P7" s="81">
+      <c r="O7" s="63"/>
+      <c r="P7" s="78">
         <v>0.6</v>
       </c>
-      <c r="Q7" s="93"/>
-      <c r="R7" s="66">
+      <c r="Q7" s="90"/>
+      <c r="R7" s="63">
         <v>0.5</v>
       </c>
-      <c r="S7" s="66"/>
-      <c r="T7" s="24"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S7" s="90"/>
+      <c r="T7" s="63">
+        <v>0.5</v>
+      </c>
+      <c r="U7" s="63"/>
+      <c r="V7" s="108"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
         <v>30</v>
       </c>
@@ -1090,23 +1119,27 @@
       <c r="K8" s="6">
         <v>0.6</v>
       </c>
-      <c r="L8" s="66"/>
-      <c r="M8" s="66"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="63"/>
       <c r="N8" s="6">
         <v>0.6</v>
       </c>
-      <c r="O8" s="66"/>
-      <c r="P8" s="81">
+      <c r="O8" s="63"/>
+      <c r="P8" s="78">
         <v>0.4</v>
       </c>
-      <c r="Q8" s="93"/>
-      <c r="R8" s="66">
+      <c r="Q8" s="90"/>
+      <c r="R8" s="63">
         <v>0.4</v>
       </c>
-      <c r="S8" s="66"/>
-      <c r="T8" s="24"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S8" s="90"/>
+      <c r="T8" s="63">
+        <v>0.5</v>
+      </c>
+      <c r="U8" s="63"/>
+      <c r="V8" s="108"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
         <v>8</v>
       </c>
@@ -1132,22 +1165,26 @@
       <c r="K9" s="4">
         <v>125001</v>
       </c>
-      <c r="L9" s="65"/>
-      <c r="M9" s="65"/>
+      <c r="L9" s="62"/>
+      <c r="M9" s="62"/>
       <c r="N9" s="4">
         <v>48000</v>
       </c>
-      <c r="O9" s="65"/>
-      <c r="P9" s="80">
+      <c r="O9" s="62"/>
+      <c r="P9" s="77">
         <v>48000</v>
       </c>
-      <c r="Q9" s="92"/>
-      <c r="R9" s="65">
+      <c r="Q9" s="89"/>
+      <c r="R9" s="62">
         <v>52000</v>
       </c>
-      <c r="S9" s="65"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S9" s="89"/>
+      <c r="T9" s="62">
+        <v>40000</v>
+      </c>
+      <c r="U9" s="62"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
         <v>51</v>
       </c>
@@ -1173,22 +1210,26 @@
       <c r="K10" s="4">
         <v>0</v>
       </c>
-      <c r="L10" s="65"/>
-      <c r="M10" s="65"/>
+      <c r="L10" s="62"/>
+      <c r="M10" s="62"/>
       <c r="N10" s="4">
         <v>0</v>
       </c>
-      <c r="O10" s="65"/>
-      <c r="P10" s="80">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="92"/>
-      <c r="R10" s="65">
+      <c r="O10" s="62"/>
+      <c r="P10" s="77">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="89"/>
+      <c r="R10" s="62">
         <v>10</v>
       </c>
-      <c r="S10" s="65"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S10" s="89"/>
+      <c r="T10" s="62">
+        <v>0</v>
+      </c>
+      <c r="U10" s="62"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
         <v>25</v>
       </c>
@@ -1212,22 +1253,26 @@
       <c r="K11" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="L11" s="65"/>
-      <c r="M11" s="65"/>
+      <c r="L11" s="62"/>
+      <c r="M11" s="62"/>
       <c r="N11" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="O11" s="65"/>
-      <c r="P11" s="80" t="b">
+      <c r="O11" s="62"/>
+      <c r="P11" s="77" t="b">
         <v>1</v>
       </c>
-      <c r="Q11" s="92"/>
-      <c r="R11" s="65" t="b">
-        <v>0</v>
-      </c>
-      <c r="S11" s="65"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="Q11" s="89"/>
+      <c r="R11" s="62" t="b">
+        <v>0</v>
+      </c>
+      <c r="S11" s="89"/>
+      <c r="T11" s="62" t="b">
+        <v>0</v>
+      </c>
+      <c r="U11" s="62"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
         <v>26</v>
       </c>
@@ -1251,25 +1296,29 @@
       <c r="K12" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="L12" s="65"/>
-      <c r="M12" s="65"/>
+      <c r="L12" s="62"/>
+      <c r="M12" s="62"/>
       <c r="N12" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="O12" s="65"/>
-      <c r="P12" s="80" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="92"/>
-      <c r="R12" s="65" t="b">
-        <v>0</v>
-      </c>
-      <c r="S12" s="65"/>
-      <c r="T12" s="11" t="s">
+      <c r="O12" s="62"/>
+      <c r="P12" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="89"/>
+      <c r="R12" s="62" t="b">
+        <v>0</v>
+      </c>
+      <c r="S12" s="89"/>
+      <c r="T12" s="62" t="b">
+        <v>0</v>
+      </c>
+      <c r="U12" s="62"/>
+      <c r="V12" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="s">
         <v>27</v>
       </c>
@@ -1293,25 +1342,29 @@
       <c r="K13" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="L13" s="65"/>
-      <c r="M13" s="65"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="62"/>
       <c r="N13" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="O13" s="65"/>
-      <c r="P13" s="80" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="92"/>
-      <c r="R13" s="65" t="b">
-        <v>0</v>
-      </c>
-      <c r="S13" s="65"/>
-      <c r="T13" s="11" t="s">
+      <c r="O13" s="62"/>
+      <c r="P13" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="89"/>
+      <c r="R13" s="62" t="b">
+        <v>0</v>
+      </c>
+      <c r="S13" s="89"/>
+      <c r="T13" s="62" t="b">
+        <v>0</v>
+      </c>
+      <c r="U13" s="62"/>
+      <c r="V13" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="C14" s="13"/>
       <c r="D14" s="15"/>
       <c r="E14" s="13"/>
@@ -1321,16 +1374,18 @@
       <c r="I14" s="13"/>
       <c r="J14" s="14"/>
       <c r="K14" s="13"/>
-      <c r="L14" s="63"/>
-      <c r="M14" s="63"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60"/>
       <c r="N14" s="13"/>
-      <c r="O14" s="63"/>
-      <c r="P14" s="78"/>
-      <c r="Q14" s="90"/>
-      <c r="R14" s="63"/>
-      <c r="S14" s="63"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="O14" s="60"/>
+      <c r="P14" s="75"/>
+      <c r="Q14" s="87"/>
+      <c r="R14" s="60"/>
+      <c r="S14" s="87"/>
+      <c r="T14" s="60"/>
+      <c r="U14" s="60"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>5</v>
       </c>
@@ -1344,16 +1399,18 @@
       <c r="I15" s="18"/>
       <c r="J15" s="19"/>
       <c r="K15" s="18"/>
-      <c r="L15" s="64"/>
-      <c r="M15" s="64"/>
+      <c r="L15" s="61"/>
+      <c r="M15" s="61"/>
       <c r="N15" s="18"/>
-      <c r="O15" s="64"/>
-      <c r="P15" s="79"/>
-      <c r="Q15" s="91"/>
-      <c r="R15" s="64"/>
-      <c r="S15" s="64"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="O15" s="61"/>
+      <c r="P15" s="76"/>
+      <c r="Q15" s="88"/>
+      <c r="R15" s="61"/>
+      <c r="S15" s="88"/>
+      <c r="T15" s="61"/>
+      <c r="U15" s="61"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>0</v>
       </c>
@@ -1384,16 +1441,20 @@
         <v>15</v>
       </c>
       <c r="O16" s="23"/>
-      <c r="P16" s="82">
+      <c r="P16" s="79">
         <v>15</v>
       </c>
-      <c r="Q16" s="94"/>
+      <c r="Q16" s="91"/>
       <c r="R16" s="23">
         <v>15</v>
       </c>
-      <c r="S16" s="23"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S16" s="91"/>
+      <c r="T16" s="23">
+        <v>15</v>
+      </c>
+      <c r="U16" s="23"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>3</v>
       </c>
@@ -1424,16 +1485,20 @@
         <v>130</v>
       </c>
       <c r="O17" s="23"/>
-      <c r="P17" s="82">
+      <c r="P17" s="79">
         <v>130</v>
       </c>
-      <c r="Q17" s="94"/>
+      <c r="Q17" s="91"/>
       <c r="R17" s="23">
         <v>130</v>
       </c>
-      <c r="S17" s="23"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S17" s="91"/>
+      <c r="T17" s="23">
+        <v>130</v>
+      </c>
+      <c r="U17" s="23"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>15</v>
       </c>
@@ -1464,16 +1529,20 @@
         <v>32</v>
       </c>
       <c r="O18" s="23"/>
-      <c r="P18" s="82">
+      <c r="P18" s="79">
         <v>32</v>
       </c>
-      <c r="Q18" s="94"/>
+      <c r="Q18" s="91"/>
       <c r="R18" s="23">
         <v>32</v>
       </c>
-      <c r="S18" s="23"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S18" s="91"/>
+      <c r="T18" s="23">
+        <v>32</v>
+      </c>
+      <c r="U18" s="23"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="C19" s="25"/>
       <c r="D19" s="15"/>
       <c r="E19" s="25"/>
@@ -1486,12 +1555,14 @@
       <c r="M19" s="23"/>
       <c r="N19" s="25"/>
       <c r="O19" s="23"/>
-      <c r="P19" s="82"/>
-      <c r="Q19" s="94"/>
+      <c r="P19" s="79"/>
+      <c r="Q19" s="91"/>
       <c r="R19" s="23"/>
-      <c r="S19" s="23"/>
-    </row>
-    <row r="20" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S19" s="91"/>
+      <c r="T19" s="23"/>
+      <c r="U19" s="23"/>
+    </row>
+    <row r="20" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
         <v>4</v>
       </c>
@@ -1505,16 +1576,18 @@
       <c r="I20" s="18"/>
       <c r="J20" s="19"/>
       <c r="K20" s="18"/>
-      <c r="L20" s="64"/>
-      <c r="M20" s="64"/>
+      <c r="L20" s="61"/>
+      <c r="M20" s="61"/>
       <c r="N20" s="18"/>
-      <c r="O20" s="64"/>
-      <c r="P20" s="79"/>
-      <c r="Q20" s="91"/>
-      <c r="R20" s="64"/>
-      <c r="S20" s="64"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="O20" s="61"/>
+      <c r="P20" s="76"/>
+      <c r="Q20" s="88"/>
+      <c r="R20" s="61"/>
+      <c r="S20" s="88"/>
+      <c r="T20" s="61"/>
+      <c r="U20" s="61"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="26" t="s">
         <v>16</v>
       </c>
@@ -1540,22 +1613,26 @@
       <c r="K21" s="27">
         <v>48000</v>
       </c>
-      <c r="L21" s="67"/>
-      <c r="M21" s="67"/>
+      <c r="L21" s="64"/>
+      <c r="M21" s="64"/>
       <c r="N21" s="27">
         <v>48000</v>
       </c>
-      <c r="O21" s="67"/>
-      <c r="P21" s="83">
+      <c r="O21" s="64"/>
+      <c r="P21" s="80">
         <v>48000</v>
       </c>
-      <c r="Q21" s="95"/>
-      <c r="R21" s="67">
+      <c r="Q21" s="92"/>
+      <c r="R21" s="64">
         <v>48000</v>
       </c>
-      <c r="S21" s="67"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S21" s="92"/>
+      <c r="T21" s="64">
+        <v>48000</v>
+      </c>
+      <c r="U21" s="64"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>6</v>
       </c>
@@ -1581,22 +1658,26 @@
       <c r="K22" s="27">
         <v>125000</v>
       </c>
-      <c r="L22" s="67"/>
-      <c r="M22" s="67"/>
+      <c r="L22" s="64"/>
+      <c r="M22" s="64"/>
       <c r="N22" s="27">
         <v>125000</v>
       </c>
-      <c r="O22" s="67"/>
-      <c r="P22" s="83">
+      <c r="O22" s="64"/>
+      <c r="P22" s="80">
         <v>125000</v>
       </c>
-      <c r="Q22" s="95"/>
-      <c r="R22" s="67">
+      <c r="Q22" s="92"/>
+      <c r="R22" s="64">
         <v>125000</v>
       </c>
-      <c r="S22" s="67"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S22" s="92"/>
+      <c r="T22" s="64">
+        <v>125000</v>
+      </c>
+      <c r="U22" s="64"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="C23" s="25"/>
       <c r="D23" s="15"/>
       <c r="E23" s="25"/>
@@ -1609,12 +1690,14 @@
       <c r="M23" s="23"/>
       <c r="N23" s="25"/>
       <c r="O23" s="23"/>
-      <c r="P23" s="82"/>
-      <c r="Q23" s="94"/>
+      <c r="P23" s="79"/>
+      <c r="Q23" s="91"/>
       <c r="R23" s="23"/>
-      <c r="S23" s="23"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S23" s="91"/>
+      <c r="T23" s="23"/>
+      <c r="U23" s="23"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
         <v>21</v>
       </c>
@@ -1628,114 +1711,125 @@
       <c r="I24" s="18"/>
       <c r="J24" s="19"/>
       <c r="K24" s="18"/>
-      <c r="L24" s="64"/>
-      <c r="M24" s="64"/>
+      <c r="L24" s="61"/>
+      <c r="M24" s="61"/>
       <c r="N24" s="18"/>
-      <c r="O24" s="64"/>
-      <c r="P24" s="79"/>
-      <c r="Q24" s="91"/>
-      <c r="R24" s="64"/>
-      <c r="S24" s="64"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="O24" s="61"/>
+      <c r="P24" s="76"/>
+      <c r="Q24" s="88"/>
+      <c r="R24" s="61"/>
+      <c r="S24" s="88"/>
+      <c r="T24" s="61"/>
+      <c r="U24" s="61"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" s="21" t="s">
         <v>57</v>
       </c>
       <c r="B25" s="21"/>
-      <c r="C25" s="60">
+      <c r="C25" s="57">
         <f>IF(C8&lt;C7,C8/C7*C6,C6)</f>
         <v>2080</v>
       </c>
-      <c r="D25" s="61"/>
-      <c r="E25" s="60">
+      <c r="D25" s="58"/>
+      <c r="E25" s="57">
         <f>IF(E8&lt;E7,E8/E7*E6,E6)</f>
         <v>1366.6666666666667</v>
       </c>
-      <c r="F25" s="61"/>
-      <c r="G25" s="60">
+      <c r="F25" s="58"/>
+      <c r="G25" s="57">
         <f>IF(G8&lt;G7,G8/G7*G6,G6)</f>
         <v>2080</v>
       </c>
-      <c r="H25" s="61"/>
-      <c r="I25" s="60">
+      <c r="H25" s="58"/>
+      <c r="I25" s="57">
         <f>IF(I8&lt;I7,I8/I7*I6,I6)</f>
         <v>1600</v>
       </c>
-      <c r="J25" s="61"/>
-      <c r="K25" s="60">
+      <c r="J25" s="58"/>
+      <c r="K25" s="57">
         <f>IF(K8&lt;K7,K8/K7*K6,K6)</f>
         <v>1600</v>
       </c>
-      <c r="L25" s="68"/>
-      <c r="M25" s="68"/>
-      <c r="N25" s="60">
+      <c r="L25" s="65"/>
+      <c r="M25" s="65"/>
+      <c r="N25" s="57">
         <f>IF(N8&lt;N7,N8/N7*N6,N6)</f>
         <v>1371.4285714285716</v>
       </c>
-      <c r="O25" s="73"/>
-      <c r="P25" s="84">
+      <c r="O25" s="70"/>
+      <c r="P25" s="81">
         <f>IF(P8&lt;P7,P8/P7*P6,P6)</f>
         <v>1066.6666666666667</v>
       </c>
-      <c r="Q25" s="96"/>
-      <c r="R25" s="73">
+      <c r="Q25" s="93"/>
+      <c r="R25" s="70">
         <f>IF(R8&lt;R7,R8/R7*R6,R6)</f>
         <v>1280</v>
       </c>
-      <c r="S25" s="73"/>
-      <c r="T25" s="24"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S25" s="93"/>
+      <c r="T25" s="70">
+        <f>IF(T8&lt;T7,T8/T7*T6,T6)</f>
+        <v>1600</v>
+      </c>
+      <c r="U25" s="70"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" s="30" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="30"/>
-      <c r="C26" s="55">
+      <c r="C26" s="53">
         <f>IF(C9&lt;=125000,((C16/C17)+((C29*(C9-C21)))),101%)</f>
         <v>0.11728896103896104</v>
       </c>
       <c r="D26" s="32"/>
-      <c r="E26" s="55">
+      <c r="E26" s="53">
         <f>IF(E9&lt;=125000,((E16/E17)+((E29*(E9-E21)))),101%)</f>
         <v>0.47037337662337664</v>
       </c>
       <c r="F26" s="32"/>
-      <c r="G26" s="55">
+      <c r="G26" s="53">
         <f>IF(G9&lt;=125000,((G16/G17)+((G29*(G9-G21)))),101%)</f>
         <v>1.01</v>
       </c>
       <c r="H26" s="32"/>
-      <c r="I26" s="55">
+      <c r="I26" s="53">
         <f>IF(((I16/I17)+((I29*(I9-I21))))&lt;=100%,((I16/I17)+((I29*(I9-I21)))),100%)</f>
         <v>0.94255744255744267</v>
       </c>
       <c r="J26" s="32"/>
-      <c r="K26" s="55">
+      <c r="K26" s="53">
         <f>IF(((K16/K17)+((K29*(K9-K21))))&lt;=100%,((K16/K17)+((K29*(K9-K21)))),100%)</f>
         <v>1</v>
       </c>
-      <c r="L26" s="69"/>
-      <c r="M26" s="69"/>
-      <c r="N26" s="55">
+      <c r="L26" s="66"/>
+      <c r="M26" s="66"/>
+      <c r="N26" s="53">
         <f>IF(((N16/N17)+((N29*(N9-N21))))&lt;=100%,((N16/N17)+((N29*(N9-N21)))),100%)</f>
         <v>0.11538461538461539</v>
       </c>
-      <c r="O26" s="74"/>
-      <c r="P26" s="85">
+      <c r="O26" s="71"/>
+      <c r="P26" s="82">
         <f>IF(((P16/P17)+((P29*(P9-P21))))&lt;=100%,((P16/P17)+((P29*(P9-P21)))),100%)</f>
         <v>0.11538461538461539</v>
       </c>
-      <c r="Q26" s="97"/>
-      <c r="R26" s="74">
+      <c r="Q26" s="94"/>
+      <c r="R26" s="71">
         <f>IF(((R16/R17)+((R29*(R9-R21))))&lt;=100%,((R16/R17)+((R29*(R9-R21)))),100%)</f>
         <v>0.16133866133866134</v>
       </c>
-      <c r="S26" s="74"/>
-      <c r="T26" s="54" t="s">
+      <c r="S26" s="94"/>
+      <c r="T26" s="71">
+        <f t="shared" ref="T26" si="0">IF(((T16/T17)+((T29*(T9-T21))))&lt;=100%,((T16/T17)+((T29*(T9-T21)))),100%)</f>
+        <v>2.3476523476523486E-2</v>
+      </c>
+      <c r="U26" s="71"/>
+      <c r="V26" s="109" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" s="34" t="s">
         <v>10</v>
       </c>
@@ -1771,22 +1865,28 @@
         <f>IF(N$9&lt;=125000,N$26*50%*N$17,0)</f>
         <v>7.5</v>
       </c>
-      <c r="O27" s="75"/>
-      <c r="P27" s="86">
+      <c r="O27" s="72"/>
+      <c r="P27" s="83">
         <f>IF(P$9&lt;=125000,P$26*50%*P$17,0)</f>
         <v>7.5</v>
       </c>
-      <c r="Q27" s="98"/>
-      <c r="R27" s="75">
+      <c r="Q27" s="95"/>
+      <c r="R27" s="72">
         <f>IF(R$9&lt;=125000,R$26*50%*R$17,0)</f>
         <v>10.487012987012987</v>
       </c>
-      <c r="S27" s="75"/>
-      <c r="T27" s="36" t="s">
+      <c r="S27" s="95"/>
+      <c r="T27" s="72">
+        <f t="shared" ref="T27" si="1">IF(T$9&lt;=125000,T$26*50%*T$17,0)</f>
+        <v>1.5259740259740266</v>
+      </c>
+      <c r="U27" s="72"/>
+      <c r="V27" s="108" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="28" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="X27" s="106"/>
+    </row>
+    <row r="28" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="34" t="s">
         <v>11</v>
       </c>
@@ -1822,22 +1922,28 @@
         <f>IF(N$9&lt;=125000,N$26*70%*N$17,0)</f>
         <v>10.5</v>
       </c>
-      <c r="O28" s="75"/>
-      <c r="P28" s="86">
+      <c r="O28" s="72"/>
+      <c r="P28" s="83">
         <f>IF(P$9&lt;=125000,P$26*70%*P$17,0)</f>
         <v>10.5</v>
       </c>
-      <c r="Q28" s="98"/>
-      <c r="R28" s="75">
+      <c r="Q28" s="95"/>
+      <c r="R28" s="72">
         <f>IF(R$9&lt;=125000,R$26*70%*R$17,0)</f>
         <v>14.681818181818182</v>
       </c>
-      <c r="S28" s="75"/>
-      <c r="T28" s="36" t="s">
+      <c r="S28" s="95"/>
+      <c r="T28" s="72">
+        <f t="shared" ref="T28" si="2">IF(T$9&lt;=125000,T$26*70%*T$17,0)</f>
+        <v>2.1363636363636371</v>
+      </c>
+      <c r="U28" s="72"/>
+      <c r="V28" s="108" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="X28" s="55"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" s="34" t="s">
         <v>9</v>
       </c>
@@ -1866,28 +1972,33 @@
         <f>((1-(K16/K17))/(K22-K21))</f>
         <v>1.1488511488511489E-5</v>
       </c>
-      <c r="L29" s="70"/>
-      <c r="M29" s="70"/>
+      <c r="L29" s="67"/>
+      <c r="M29" s="67"/>
       <c r="N29" s="38">
         <f>((1-(N16/N17))/(N22-N21))</f>
         <v>1.1488511488511489E-5</v>
       </c>
-      <c r="O29" s="76"/>
-      <c r="P29" s="87">
+      <c r="O29" s="73"/>
+      <c r="P29" s="84">
         <f>((1-(P16/P17))/(P22-P21))</f>
         <v>1.1488511488511489E-5</v>
       </c>
-      <c r="Q29" s="99"/>
-      <c r="R29" s="76">
+      <c r="Q29" s="96"/>
+      <c r="R29" s="73">
         <f>((1-(R16/R17))/(R22-R21))</f>
         <v>1.1488511488511489E-5</v>
       </c>
-      <c r="S29" s="76"/>
-      <c r="T29" s="22" t="s">
+      <c r="S29" s="96"/>
+      <c r="T29" s="73">
+        <f t="shared" ref="T29" si="3">((1-(T16/T17))/(T22-T21))</f>
+        <v>1.1488511488511489E-5</v>
+      </c>
+      <c r="U29" s="73"/>
+      <c r="V29" s="107" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" s="34" t="s">
         <v>53</v>
       </c>
@@ -1911,23 +2022,27 @@
       <c r="K30" s="35">
         <v>10</v>
       </c>
-      <c r="L30" s="70"/>
-      <c r="M30" s="70"/>
+      <c r="L30" s="67"/>
+      <c r="M30" s="67"/>
       <c r="N30" s="35">
         <v>10</v>
       </c>
-      <c r="O30" s="75"/>
-      <c r="P30" s="86">
-        <v>11</v>
-      </c>
-      <c r="Q30" s="98"/>
-      <c r="R30" s="75">
-        <v>11</v>
-      </c>
-      <c r="S30" s="75"/>
-      <c r="T30" s="22"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="O30" s="72"/>
+      <c r="P30" s="35">
+        <v>10</v>
+      </c>
+      <c r="Q30" s="95"/>
+      <c r="R30" s="35">
+        <v>10</v>
+      </c>
+      <c r="S30" s="95"/>
+      <c r="T30" s="35">
+        <v>10</v>
+      </c>
+      <c r="U30" s="72"/>
+      <c r="V30" s="107"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" s="34" t="s">
         <v>31</v>
       </c>
@@ -1956,26 +2071,32 @@
         <f>MIN(K7:K8)</f>
         <v>0.6</v>
       </c>
-      <c r="L31" s="70"/>
-      <c r="M31" s="70"/>
+      <c r="L31" s="67"/>
+      <c r="M31" s="67"/>
       <c r="N31" s="31">
         <f>MIN(N7:N8)</f>
         <v>0.6</v>
       </c>
-      <c r="O31" s="77"/>
-      <c r="P31" s="88">
+      <c r="O31" s="74"/>
+      <c r="P31" s="85">
         <f>MIN(P7:P8)</f>
         <v>0.4</v>
       </c>
-      <c r="Q31" s="100"/>
-      <c r="R31" s="77">
+      <c r="Q31" s="97"/>
+      <c r="R31" s="74">
         <f>MIN(R7:R8)</f>
         <v>0.4</v>
       </c>
-      <c r="S31" s="77"/>
-      <c r="T31" s="22"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S31" s="97"/>
+      <c r="T31" s="74">
+        <f t="shared" ref="T31" si="4">MIN(T7:T8)</f>
+        <v>0.5</v>
+      </c>
+      <c r="U31" s="74"/>
+      <c r="V31" s="107"/>
+      <c r="X31" s="104"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" s="34" t="s">
         <v>14</v>
       </c>
@@ -2010,19 +2131,25 @@
         <v>3</v>
       </c>
       <c r="O32" s="23"/>
-      <c r="P32" s="82">
-        <f t="shared" ref="P32" si="0">P31*5</f>
+      <c r="P32" s="79">
+        <f t="shared" ref="P32" si="5">P31*5</f>
         <v>2</v>
       </c>
-      <c r="Q32" s="94"/>
+      <c r="Q32" s="91"/>
       <c r="R32" s="23">
-        <f t="shared" ref="R32" si="1">R31*5</f>
+        <f t="shared" ref="R32" si="6">R31*5</f>
         <v>2</v>
       </c>
-      <c r="S32" s="23"/>
-      <c r="T32" s="22"/>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S32" s="91"/>
+      <c r="T32" s="23">
+        <f t="shared" ref="T32" si="7">T31*5</f>
+        <v>2.5</v>
+      </c>
+      <c r="U32" s="23"/>
+      <c r="V32" s="107"/>
+      <c r="X32" s="105"/>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>12</v>
       </c>
@@ -2050,17 +2177,22 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="O33" s="23"/>
-      <c r="P33" s="82">
+      <c r="P33" s="79">
         <v>4.0999999999999996</v>
       </c>
-      <c r="Q33" s="94"/>
+      <c r="Q33" s="91"/>
       <c r="R33" s="23">
         <v>4.0999999999999996</v>
       </c>
-      <c r="S33" s="23"/>
-      <c r="T33" s="22"/>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S33" s="91"/>
+      <c r="T33" s="23">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="U33" s="23"/>
+      <c r="V33" s="107"/>
+      <c r="X33" s="55"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>24</v>
       </c>
@@ -2094,18 +2226,23 @@
         <v>12.299999999999999</v>
       </c>
       <c r="O34" s="23"/>
-      <c r="P34" s="82">
+      <c r="P34" s="79">
         <f>P32*P33</f>
         <v>8.1999999999999993</v>
       </c>
-      <c r="Q34" s="94"/>
+      <c r="Q34" s="91"/>
       <c r="R34" s="23">
         <f>R32*R33</f>
         <v>8.1999999999999993</v>
       </c>
-      <c r="S34" s="23"/>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S34" s="91"/>
+      <c r="T34" s="23">
+        <f t="shared" ref="T34" si="8">T32*T33</f>
+        <v>10.25</v>
+      </c>
+      <c r="U34" s="23"/>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="34"/>
       <c r="B35" s="34"/>
       <c r="C35" s="38"/>
@@ -2117,17 +2254,20 @@
       <c r="I35" s="38"/>
       <c r="J35" s="39"/>
       <c r="K35" s="38"/>
-      <c r="L35" s="70"/>
-      <c r="M35" s="70"/>
+      <c r="L35" s="67"/>
+      <c r="M35" s="67"/>
       <c r="N35" s="38"/>
-      <c r="O35" s="76"/>
-      <c r="P35" s="87"/>
-      <c r="Q35" s="99"/>
-      <c r="R35" s="76"/>
-      <c r="S35" s="76"/>
-      <c r="T35" s="22"/>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="O35" s="73"/>
+      <c r="P35" s="84"/>
+      <c r="Q35" s="96"/>
+      <c r="R35" s="73"/>
+      <c r="S35" s="96"/>
+      <c r="T35" s="73"/>
+      <c r="U35" s="73"/>
+      <c r="V35" s="107"/>
+      <c r="X35" s="104"/>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" s="16" t="s">
         <v>47</v>
       </c>
@@ -2141,16 +2281,19 @@
       <c r="I36" s="18"/>
       <c r="J36" s="19"/>
       <c r="K36" s="18"/>
-      <c r="L36" s="64"/>
-      <c r="M36" s="64"/>
+      <c r="L36" s="61"/>
+      <c r="M36" s="61"/>
       <c r="N36" s="18"/>
-      <c r="O36" s="64"/>
-      <c r="P36" s="79"/>
-      <c r="Q36" s="91"/>
-      <c r="R36" s="64"/>
-      <c r="S36" s="64"/>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="O36" s="61"/>
+      <c r="P36" s="76"/>
+      <c r="Q36" s="88"/>
+      <c r="R36" s="61"/>
+      <c r="S36" s="88"/>
+      <c r="T36" s="61"/>
+      <c r="U36" s="61"/>
+      <c r="X36" s="105"/>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" s="34" t="s">
         <v>23</v>
       </c>
@@ -2158,48 +2301,58 @@
         <v>49</v>
       </c>
       <c r="C37" s="40">
-        <f>IF((C17*(1-C26))&gt;C30,(C17*(1-C26)),IF(C26&lt;=100%,C30,IF(C26&gt;100%,0)))</f>
-        <v>141.23376623376623</v>
-      </c>
-      <c r="D37" s="41"/>
+        <v>141.233766233766</v>
+      </c>
+      <c r="D37" s="40"/>
       <c r="E37" s="40">
-        <f>IF((E17*(1-E26))&gt;E30,(E17*(1-E26)),IF(E26&lt;=100%,E30,IF(E26&gt;100%,0)))</f>
+        <f t="shared" ref="E37:P37" si="9">MIN((IF((E17*(1-E26))&gt;E30,(E17*(1-E26)),IF(E26&lt;=100%,E30,IF(E26&gt;100%,0)))),E17-E16)</f>
         <v>84.740259740259745</v>
       </c>
-      <c r="F37" s="41"/>
+      <c r="F37" s="40"/>
       <c r="G37" s="40">
-        <f>IF((G17*(1-G26))&gt;G30,(G17*(1-G26)),IF(G26&lt;=100%,G30,IF(G26&gt;100%,0)))</f>
-        <v>0</v>
-      </c>
-      <c r="H37" s="41"/>
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H37" s="40"/>
       <c r="I37" s="40">
-        <f>IF((I17*(1-I26))&gt;I30,(I17*(1-I26)),IF(I9&lt;=125000,I30,0))</f>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
-      <c r="J37" s="41"/>
+      <c r="J37" s="40"/>
       <c r="K37" s="40">
-        <f>IF((K17*(1-K26))&gt;K30,(K17*(1-K26)),IF(K9&lt;=125000,K30,0))</f>
-        <v>0</v>
-      </c>
-      <c r="L37" s="71"/>
-      <c r="M37" s="71"/>
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="L37" s="40"/>
+      <c r="M37" s="40">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
       <c r="N37" s="40">
-        <f>IF((N17*(1-N26))&gt;N30,(N17*(1-N26)),IF(N9&lt;=125000,N30,0))</f>
+        <f t="shared" si="9"/>
         <v>115</v>
       </c>
-      <c r="O37" s="71"/>
-      <c r="P37" s="89">
-        <f>IF((P17*(1-P26))&gt;P30,(P17*(1-P26)),IF(P9&lt;=125000,P30,0))</f>
+      <c r="O37" s="40"/>
+      <c r="P37" s="40">
+        <f t="shared" si="9"/>
         <v>115</v>
       </c>
-      <c r="Q37" s="101"/>
-      <c r="R37" s="71">
-        <f>IF((R17*(1-R26))&gt;R30,(R17*(1-R26)),IF(R9&lt;=125000,R30,0))</f>
+      <c r="Q37" s="40"/>
+      <c r="R37" s="40">
+        <f>MIN((IF((R17*(1-R26))&gt;R30,(R17*(1-R26)),IF(R26&lt;=100%,R30,IF(R26&gt;100%,0)))),R17-R16)</f>
         <v>109.02597402597402</v>
       </c>
-      <c r="S37" s="71"/>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S37" s="98"/>
+      <c r="T37" s="68">
+        <f>MIN((IF((T17*(1-T26))&gt;T30,(T17*(1-T26)),IF(T26&lt;=100%,T30,IF(T26&gt;100%,0)))),T17-T16)</f>
+        <v>115</v>
+      </c>
+      <c r="U37" s="68"/>
+      <c r="V37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" s="34" t="str">
         <f>A12</f>
         <v>Geschwisternbonus 2. Kind</v>
@@ -2231,26 +2384,30 @@
         <f>IF(K12,K27,0)</f>
         <v>0</v>
       </c>
-      <c r="L38" s="71"/>
-      <c r="M38" s="71"/>
+      <c r="L38" s="68"/>
+      <c r="M38" s="68"/>
       <c r="N38" s="40">
         <f>IF(N12,N27,0)</f>
         <v>0</v>
       </c>
-      <c r="O38" s="71"/>
-      <c r="P38" s="89">
+      <c r="O38" s="68"/>
+      <c r="P38" s="86">
         <f>IF(P12,P27,0)</f>
         <v>0</v>
       </c>
-      <c r="Q38" s="101"/>
-      <c r="R38" s="71">
+      <c r="Q38" s="98"/>
+      <c r="R38" s="68">
         <f>IF(R12,R27,0)</f>
         <v>0</v>
       </c>
-      <c r="S38" s="71"/>
-      <c r="T38" s="56"/>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S38" s="98"/>
+      <c r="T38" s="68">
+        <f t="shared" ref="T38" si="10">IF(T12,T27,0)</f>
+        <v>0</v>
+      </c>
+      <c r="U38" s="68"/>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" s="34" t="str">
         <f>A13</f>
         <v>Geschwisternbonus 3. Kind</v>
@@ -2282,26 +2439,31 @@
         <f>IF(K13,K28,0)</f>
         <v>0</v>
       </c>
-      <c r="L39" s="71"/>
-      <c r="M39" s="71"/>
+      <c r="L39" s="68"/>
+      <c r="M39" s="68"/>
       <c r="N39" s="40">
         <f>IF(N13,N28,0)</f>
         <v>0</v>
       </c>
-      <c r="O39" s="71"/>
-      <c r="P39" s="89">
+      <c r="O39" s="68"/>
+      <c r="P39" s="86">
         <f>IF(P13,P28,0)</f>
         <v>0</v>
       </c>
-      <c r="Q39" s="101"/>
-      <c r="R39" s="71">
+      <c r="Q39" s="98"/>
+      <c r="R39" s="68">
         <f>IF(R13,R28,0)</f>
         <v>0</v>
       </c>
-      <c r="S39" s="71"/>
-      <c r="T39" s="22"/>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S39" s="98"/>
+      <c r="T39" s="68">
+        <f t="shared" ref="T39" si="11">IF(T13,T28,0)</f>
+        <v>0</v>
+      </c>
+      <c r="U39" s="68"/>
+      <c r="V39" s="107"/>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" s="43" t="s">
         <v>42</v>
       </c>
@@ -2310,7 +2472,7 @@
       </c>
       <c r="C40" s="40">
         <f>C39+C38+C37</f>
-        <v>141.23376623376623</v>
+        <v>141.233766233766</v>
       </c>
       <c r="D40" s="41"/>
       <c r="E40" s="40">
@@ -2330,27 +2492,32 @@
       <c r="J40" s="41"/>
       <c r="K40" s="40">
         <f>K39+K38+K37</f>
-        <v>0</v>
-      </c>
-      <c r="L40" s="71"/>
-      <c r="M40" s="71"/>
+        <v>10</v>
+      </c>
+      <c r="L40" s="68"/>
+      <c r="M40" s="68"/>
       <c r="N40" s="40">
         <f>N39+N38+N37</f>
         <v>115</v>
       </c>
-      <c r="O40" s="71"/>
-      <c r="P40" s="89">
+      <c r="O40" s="68"/>
+      <c r="P40" s="86">
         <f>P39+P38+P37</f>
         <v>115</v>
       </c>
-      <c r="Q40" s="101"/>
-      <c r="R40" s="71">
+      <c r="Q40" s="98"/>
+      <c r="R40" s="68">
         <f>R39+R38+R37</f>
         <v>109.02597402597402</v>
       </c>
-      <c r="S40" s="71"/>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S40" s="98"/>
+      <c r="T40" s="68">
+        <f t="shared" ref="T40" si="12">T39+T38+T37</f>
+        <v>115</v>
+      </c>
+      <c r="U40" s="68"/>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" s="44" t="s">
         <v>41</v>
       </c>
@@ -2359,7 +2526,7 @@
       </c>
       <c r="C41" s="40">
         <f>C40*C34</f>
-        <v>2316.2337662337659</v>
+        <v>2316.2337662337623</v>
       </c>
       <c r="D41" s="41"/>
       <c r="E41" s="40">
@@ -2379,27 +2546,33 @@
       <c r="J41" s="41"/>
       <c r="K41" s="40">
         <f>K40*K34</f>
-        <v>0</v>
-      </c>
-      <c r="L41" s="71"/>
-      <c r="M41" s="71"/>
+        <v>122.99999999999999</v>
+      </c>
+      <c r="L41" s="68"/>
+      <c r="M41" s="68"/>
       <c r="N41" s="40">
         <f>N40*N34</f>
         <v>1414.4999999999998</v>
       </c>
-      <c r="O41" s="71"/>
-      <c r="P41" s="89">
+      <c r="O41" s="68"/>
+      <c r="P41" s="86">
         <f>P40*P34</f>
         <v>942.99999999999989</v>
       </c>
-      <c r="Q41" s="101"/>
-      <c r="R41" s="71">
+      <c r="Q41" s="98"/>
+      <c r="R41" s="68">
         <f>R40*R34</f>
         <v>894.01298701298686</v>
       </c>
-      <c r="S41" s="71"/>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S41" s="98"/>
+      <c r="T41" s="68">
+        <f t="shared" ref="T41" si="13">T40*T34</f>
+        <v>1178.75</v>
+      </c>
+      <c r="U41" s="68"/>
+      <c r="X41" s="37"/>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" s="34" t="s">
         <v>33</v>
       </c>
@@ -2408,7 +2581,7 @@
       </c>
       <c r="C42" s="40">
         <f>C25-C41</f>
-        <v>-236.23376623376589</v>
+        <v>-236.23376623376225</v>
       </c>
       <c r="D42" s="41"/>
       <c r="E42" s="40">
@@ -2428,27 +2601,32 @@
       <c r="J42" s="41"/>
       <c r="K42" s="40">
         <f>K25-K41</f>
-        <v>1600</v>
-      </c>
-      <c r="L42" s="71"/>
-      <c r="M42" s="71"/>
+        <v>1477</v>
+      </c>
+      <c r="L42" s="68"/>
+      <c r="M42" s="68"/>
       <c r="N42" s="40">
         <f>N25-N41</f>
         <v>-43.071428571428214</v>
       </c>
-      <c r="O42" s="71"/>
-      <c r="P42" s="89">
+      <c r="O42" s="68"/>
+      <c r="P42" s="86">
         <f>P25-P41</f>
         <v>123.66666666666686</v>
       </c>
-      <c r="Q42" s="101"/>
-      <c r="R42" s="71">
+      <c r="Q42" s="98"/>
+      <c r="R42" s="68">
         <f>R25-R41</f>
         <v>385.98701298701314</v>
       </c>
-      <c r="S42" s="71"/>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S42" s="98"/>
+      <c r="T42" s="68">
+        <f t="shared" ref="T42" si="14">T25-T41</f>
+        <v>421.25</v>
+      </c>
+      <c r="U42" s="68"/>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" s="34" t="s">
         <v>36</v>
       </c>
@@ -2479,28 +2657,30 @@
         <f>K16*K34</f>
         <v>184.49999999999997</v>
       </c>
-      <c r="L43" s="71"/>
-      <c r="M43" s="71"/>
+      <c r="L43" s="68"/>
+      <c r="M43" s="68"/>
       <c r="N43" s="40">
         <f>N16*N34</f>
         <v>184.49999999999997</v>
       </c>
-      <c r="O43" s="71"/>
-      <c r="P43" s="89">
+      <c r="O43" s="68"/>
+      <c r="P43" s="86">
         <f>P16*P34</f>
         <v>122.99999999999999</v>
       </c>
-      <c r="Q43" s="101"/>
-      <c r="R43" s="71">
+      <c r="Q43" s="98"/>
+      <c r="R43" s="68">
         <f>R16*R34</f>
         <v>122.99999999999999</v>
       </c>
-      <c r="S43" s="71"/>
-      <c r="T43" s="53" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S43" s="98"/>
+      <c r="T43" s="68">
+        <f>T16*T34</f>
+        <v>153.75</v>
+      </c>
+      <c r="U43" s="68"/>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44" s="34" t="s">
         <v>40</v>
       </c>
@@ -2509,7 +2689,7 @@
       </c>
       <c r="C44" s="40">
         <f>IF((C43-C42)&gt;=0,(C43-C42),0)</f>
-        <v>482.23376623376589</v>
+        <v>482.23376623376225</v>
       </c>
       <c r="D44" s="41"/>
       <c r="E44" s="40">
@@ -2531,25 +2711,33 @@
         <f>IF((K43-K42)&gt;=0,(K43-K42),0)</f>
         <v>0</v>
       </c>
-      <c r="L44" s="71"/>
-      <c r="M44" s="71"/>
+      <c r="L44" s="68"/>
+      <c r="M44" s="68"/>
       <c r="N44" s="40">
         <f>IF((N43-N42)&gt;=0,(N43-N42),0)</f>
         <v>227.57142857142819</v>
       </c>
-      <c r="O44" s="71"/>
-      <c r="P44" s="89">
+      <c r="O44" s="68"/>
+      <c r="P44" s="86">
         <f>IF((P43-P42)&gt;=0,(P43-P42),0)</f>
         <v>0</v>
       </c>
-      <c r="Q44" s="101"/>
-      <c r="R44" s="71">
+      <c r="Q44" s="98"/>
+      <c r="R44" s="68">
         <f>IF((R43-R42)&gt;=0,(R43-R42),0)</f>
         <v>0</v>
       </c>
-      <c r="S44" s="71"/>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S44" s="98"/>
+      <c r="T44" s="68">
+        <f t="shared" ref="T44" si="15">IF((T43-T42)&gt;=0,(T43-T42),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U44" s="68"/>
+      <c r="V44" s="110" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45" s="44" t="s">
         <v>43</v>
       </c>
@@ -2578,27 +2766,32 @@
       <c r="J45" s="41"/>
       <c r="K45" s="40">
         <f>K41-K44</f>
-        <v>0</v>
-      </c>
-      <c r="L45" s="71"/>
-      <c r="M45" s="71"/>
+        <v>122.99999999999999</v>
+      </c>
+      <c r="L45" s="68"/>
+      <c r="M45" s="68"/>
       <c r="N45" s="40">
         <f>N41-N44</f>
         <v>1186.9285714285716</v>
       </c>
-      <c r="O45" s="71"/>
-      <c r="P45" s="89">
+      <c r="O45" s="68"/>
+      <c r="P45" s="86">
         <f>P41-P44</f>
         <v>942.99999999999989</v>
       </c>
-      <c r="Q45" s="101"/>
-      <c r="R45" s="71">
+      <c r="Q45" s="98"/>
+      <c r="R45" s="68">
         <f>R41-R44</f>
         <v>894.01298701298686</v>
       </c>
-      <c r="S45" s="71"/>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S45" s="98"/>
+      <c r="T45" s="68">
+        <f t="shared" ref="T45" si="16">T41-T44</f>
+        <v>1178.75</v>
+      </c>
+      <c r="U45" s="68"/>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" s="34" t="s">
         <v>28</v>
       </c>
@@ -2629,25 +2822,30 @@
         <f>K10</f>
         <v>0</v>
       </c>
-      <c r="L46" s="71"/>
-      <c r="M46" s="71"/>
+      <c r="L46" s="68"/>
+      <c r="M46" s="68"/>
       <c r="N46" s="40">
         <f>N10</f>
         <v>0</v>
       </c>
-      <c r="O46" s="71"/>
-      <c r="P46" s="89">
+      <c r="O46" s="68"/>
+      <c r="P46" s="86">
         <f>P10</f>
         <v>0</v>
       </c>
-      <c r="Q46" s="101"/>
-      <c r="R46" s="71">
+      <c r="Q46" s="98"/>
+      <c r="R46" s="68">
         <f>R10</f>
         <v>10</v>
       </c>
-      <c r="S46" s="71"/>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S46" s="98"/>
+      <c r="T46" s="68">
+        <f t="shared" ref="T46" si="17">T10</f>
+        <v>0</v>
+      </c>
+      <c r="U46" s="68"/>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" s="21" t="s">
         <v>29</v>
       </c>
@@ -2678,25 +2876,30 @@
         <f>IF(K11,K18,0)</f>
         <v>0</v>
       </c>
-      <c r="L47" s="71"/>
-      <c r="M47" s="71"/>
+      <c r="L47" s="68"/>
+      <c r="M47" s="68"/>
       <c r="N47" s="40">
         <f>IF(N11,N18,0)</f>
         <v>0</v>
       </c>
-      <c r="O47" s="71"/>
-      <c r="P47" s="89">
+      <c r="O47" s="68"/>
+      <c r="P47" s="86">
         <f>IF(P11,P18,0)</f>
         <v>32</v>
       </c>
-      <c r="Q47" s="101"/>
-      <c r="R47" s="71">
+      <c r="Q47" s="98"/>
+      <c r="R47" s="68">
         <f>IF(R11,R18,0)</f>
         <v>0</v>
       </c>
-      <c r="S47" s="71"/>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S47" s="98"/>
+      <c r="T47" s="68">
+        <f t="shared" ref="T47" si="18">IF(T11,T18,0)</f>
+        <v>0</v>
+      </c>
+      <c r="U47" s="68"/>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48" s="34" t="s">
         <v>37</v>
       </c>
@@ -2727,25 +2930,30 @@
         <f>(K46+K47)*K34</f>
         <v>0</v>
       </c>
-      <c r="L48" s="71"/>
-      <c r="M48" s="71"/>
+      <c r="L48" s="68"/>
+      <c r="M48" s="68"/>
       <c r="N48" s="40">
         <f>(N46+N47)*N34</f>
         <v>0</v>
       </c>
-      <c r="O48" s="71"/>
-      <c r="P48" s="89">
+      <c r="O48" s="68"/>
+      <c r="P48" s="86">
         <f>(P46+P47)*P34</f>
         <v>262.39999999999998</v>
       </c>
-      <c r="Q48" s="101"/>
-      <c r="R48" s="71">
+      <c r="Q48" s="98"/>
+      <c r="R48" s="68">
         <f>(R46+R47)*R34</f>
         <v>82</v>
       </c>
-      <c r="S48" s="71"/>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S48" s="98"/>
+      <c r="T48" s="68">
+        <f t="shared" ref="T48" si="19">(T46+T47)*T34</f>
+        <v>0</v>
+      </c>
+      <c r="U48" s="68"/>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49" s="45" t="s">
         <v>44</v>
       </c>
@@ -2774,10 +2982,10 @@
       <c r="J49" s="47"/>
       <c r="K49" s="46">
         <f>K45+K48</f>
-        <v>0</v>
-      </c>
-      <c r="L49" s="72"/>
-      <c r="M49" s="72"/>
+        <v>122.99999999999999</v>
+      </c>
+      <c r="L49" s="69"/>
+      <c r="M49" s="69"/>
       <c r="N49" s="46">
         <f>N45+N48</f>
         <v>1186.9285714285716</v>
@@ -2787,240 +2995,276 @@
         <f>P45+P48</f>
         <v>1205.3999999999999</v>
       </c>
-      <c r="Q49" s="102"/>
-      <c r="R49" s="72">
+      <c r="Q49" s="99"/>
+      <c r="R49" s="69">
         <f>R45+R48</f>
         <v>976.01298701298686</v>
       </c>
-      <c r="S49" s="46"/>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S49" s="99"/>
+      <c r="T49" s="69">
+        <f t="shared" ref="T49" si="20">T45+T48</f>
+        <v>1178.75</v>
+      </c>
+      <c r="U49" s="46"/>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="58">
+      <c r="C50" s="55">
         <f>IF((C34*(C38+C39))&lt;C49,(C34*(C38+C39)),(C49-(C37*C34)))</f>
         <v>0</v>
       </c>
-      <c r="E50" s="58">
+      <c r="E50" s="55">
         <f>IF((E34*(E38+E39))&lt;E49,(E34*(E38+E39)),(E49-(E37*E34)))</f>
         <v>0</v>
       </c>
-      <c r="G50" s="58">
+      <c r="G50" s="55">
         <f>IF((G34*(G38+G39))&lt;G49,(G34*(G38+G39)),(G49-(G37*G34)))</f>
         <v>0</v>
       </c>
-      <c r="I50" s="58">
+      <c r="I50" s="55">
         <f>IF((I34*(I38+I39))&lt;I49,(I34*(I38+I39)),(I49-(I37*I34)))</f>
         <v>0</v>
       </c>
-      <c r="K50" s="58">
+      <c r="K50" s="55">
         <f>IF((K34*(K38+K39))&lt;K49,(K34*(K38+K39)),(K49-(K37*K34)))</f>
         <v>0</v>
       </c>
-      <c r="N50" s="58">
+      <c r="N50" s="55">
         <f>IF((N34*(N38+N39))&lt;N49,(N34*(N38+N39)),(N49-(N37*N34)))</f>
         <v>0</v>
       </c>
-      <c r="O50" s="58"/>
-      <c r="P50" s="103">
+      <c r="O50" s="55"/>
+      <c r="P50" s="100">
         <f>IF((P34*(P38+P39))&lt;P49,(P34*(P38+P39)),(P49-(P37*P34)))</f>
         <v>0</v>
       </c>
-      <c r="Q50" s="104"/>
-      <c r="R50" s="58">
+      <c r="Q50" s="101"/>
+      <c r="R50" s="55">
         <f>IF((R34*(R38+R39))&lt;R49,(R34*(R38+R39)),(R49-(R37*R34)))</f>
         <v>0</v>
       </c>
-      <c r="S50" s="58"/>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="P51" s="105"/>
-      <c r="Q51" s="94"/>
+      <c r="S50" s="101"/>
+      <c r="T50" s="55">
+        <f t="shared" ref="T50" si="21">IF((T34*(T38+T39))&lt;T49,(T34*(T38+T39)),(T49-(T37*T34)))</f>
+        <v>0</v>
+      </c>
+      <c r="U50" s="55"/>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="P51" s="102"/>
+      <c r="Q51" s="91"/>
       <c r="R51"/>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C52" s="59"/>
-      <c r="P52" s="105"/>
-      <c r="Q52" s="94"/>
+      <c r="S51" s="91"/>
+      <c r="T51"/>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="C52" s="56"/>
+      <c r="P52" s="102"/>
+      <c r="Q52" s="91"/>
       <c r="R52"/>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S52" s="91"/>
+      <c r="T52"/>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>60</v>
       </c>
       <c r="B53"/>
-      <c r="C53" s="62">
+      <c r="C53" s="59">
         <f>SUM(C48,C41)</f>
-        <v>2316.2337662337659</v>
-      </c>
-      <c r="D53" s="62"/>
-      <c r="E53" s="62">
-        <f t="shared" ref="E53:K53" si="2">SUM(E48,E41)</f>
+        <v>2316.2337662337623</v>
+      </c>
+      <c r="D53" s="59"/>
+      <c r="E53" s="59">
+        <f t="shared" ref="E53:K53" si="22">SUM(E48,E41)</f>
         <v>1196.5876623376626</v>
       </c>
-      <c r="F53" s="62"/>
-      <c r="G53" s="62">
-        <f t="shared" ref="G53" si="3">SUM(G48,G41)</f>
-        <v>0</v>
-      </c>
-      <c r="H53" s="62"/>
-      <c r="I53" s="62">
-        <f t="shared" si="2"/>
+      <c r="F53" s="59"/>
+      <c r="G53" s="59">
+        <f t="shared" ref="G53" si="23">SUM(G48,G41)</f>
+        <v>0</v>
+      </c>
+      <c r="H53" s="59"/>
+      <c r="I53" s="59">
+        <f t="shared" si="22"/>
         <v>122.99999999999999</v>
       </c>
-      <c r="J53" s="62"/>
-      <c r="K53" s="62">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N53" s="62">
-        <f t="shared" ref="N53" si="4">SUM(N48,N41)</f>
+      <c r="J53" s="59"/>
+      <c r="K53" s="59">
+        <f t="shared" si="22"/>
+        <v>122.99999999999999</v>
+      </c>
+      <c r="N53" s="59">
+        <f t="shared" ref="N53" si="24">SUM(N48,N41)</f>
         <v>1414.4999999999998</v>
       </c>
-      <c r="O53" s="62"/>
-      <c r="P53" s="106">
+      <c r="O53" s="59"/>
+      <c r="P53" s="103">
         <f>SUM(P48,P41)</f>
         <v>1205.3999999999999</v>
       </c>
-      <c r="Q53" s="94"/>
-      <c r="R53" s="62">
+      <c r="Q53" s="91"/>
+      <c r="R53" s="59">
         <f>SUM(R48,R41)</f>
         <v>976.01298701298686</v>
       </c>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S53" s="91"/>
+      <c r="T53" s="59">
+        <f t="shared" ref="T53" si="25">SUM(T48,T41)</f>
+        <v>1178.75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>61</v>
       </c>
       <c r="B54"/>
-      <c r="C54" s="62">
+      <c r="C54" s="59">
         <f>IF(C42&lt;0,C41+C42,C41)+C48</f>
         <v>2080</v>
       </c>
-      <c r="D54" s="62"/>
-      <c r="E54" s="62">
-        <f t="shared" ref="E54:K54" si="5">IF(E42&lt;0,E41+E42,E41)+E48</f>
+      <c r="D54" s="59"/>
+      <c r="E54" s="59">
+        <f t="shared" ref="E54:K54" si="26">IF(E42&lt;0,E41+E42,E41)+E48</f>
         <v>1196.5876623376626</v>
       </c>
-      <c r="F54" s="62"/>
-      <c r="G54" s="62">
-        <f t="shared" ref="G54" si="6">IF(G42&lt;0,G41+G42,G41)+G48</f>
-        <v>0</v>
-      </c>
-      <c r="H54" s="62"/>
-      <c r="I54" s="62">
-        <f t="shared" si="5"/>
+      <c r="F54" s="59"/>
+      <c r="G54" s="59">
+        <f t="shared" ref="G54" si="27">IF(G42&lt;0,G41+G42,G41)+G48</f>
+        <v>0</v>
+      </c>
+      <c r="H54" s="59"/>
+      <c r="I54" s="59">
+        <f t="shared" si="26"/>
         <v>122.99999999999999</v>
       </c>
-      <c r="J54" s="62"/>
-      <c r="K54" s="62">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N54" s="62">
-        <f t="shared" ref="N54" si="7">IF(N42&lt;0,N41+N42,N41)+N48</f>
+      <c r="J54" s="59"/>
+      <c r="K54" s="59">
+        <f t="shared" si="26"/>
+        <v>122.99999999999999</v>
+      </c>
+      <c r="N54" s="59">
+        <f t="shared" ref="N54" si="28">IF(N42&lt;0,N41+N42,N41)+N48</f>
         <v>1371.4285714285716</v>
       </c>
-      <c r="O54" s="62"/>
-      <c r="P54" s="106">
+      <c r="O54" s="59"/>
+      <c r="P54" s="103">
         <f>IF(P42&lt;0,P41+P42,P41)+P48</f>
         <v>1205.3999999999999</v>
       </c>
-      <c r="Q54" s="94"/>
-      <c r="R54" s="62">
+      <c r="Q54" s="91"/>
+      <c r="R54" s="59">
         <f>IF(R42&lt;0,R41+R42,R41)+R48</f>
         <v>976.01298701298686</v>
       </c>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S54" s="91"/>
+      <c r="T54" s="59">
+        <f t="shared" ref="T54" si="29">IF(T42&lt;0,T41+T42,T41)+T48</f>
+        <v>1178.75</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>58</v>
       </c>
       <c r="B55"/>
-      <c r="C55" s="62">
+      <c r="C55" s="59">
         <f>IF(C43&gt;C44,C44,C43)</f>
         <v>245.99999999999997</v>
       </c>
-      <c r="D55" s="62"/>
-      <c r="E55" s="62">
-        <f t="shared" ref="E55:K55" si="8">IF(E43&gt;E44,E44,E43)</f>
-        <v>0</v>
-      </c>
-      <c r="F55" s="62"/>
-      <c r="G55" s="62">
-        <f t="shared" ref="G55" si="9">IF(G43&gt;G44,G44,G43)</f>
-        <v>0</v>
-      </c>
-      <c r="H55" s="62"/>
-      <c r="I55" s="62">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="J55" s="62"/>
-      <c r="K55" s="62">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="N55" s="62">
-        <f t="shared" ref="N55" si="10">IF(N43&gt;N44,N44,N43)</f>
+      <c r="D55" s="59"/>
+      <c r="E55" s="59">
+        <f t="shared" ref="E55:K55" si="30">IF(E43&gt;E44,E44,E43)</f>
+        <v>0</v>
+      </c>
+      <c r="F55" s="59"/>
+      <c r="G55" s="59">
+        <f t="shared" ref="G55" si="31">IF(G43&gt;G44,G44,G43)</f>
+        <v>0</v>
+      </c>
+      <c r="H55" s="59"/>
+      <c r="I55" s="59">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="J55" s="59"/>
+      <c r="K55" s="59">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="N55" s="59">
+        <f t="shared" ref="N55" si="32">IF(N43&gt;N44,N44,N43)</f>
         <v>184.49999999999997</v>
       </c>
-      <c r="O55" s="62"/>
-      <c r="P55" s="106">
+      <c r="O55" s="59"/>
+      <c r="P55" s="103">
         <f>IF(P43&gt;P44,P44,P43)</f>
         <v>0</v>
       </c>
-      <c r="Q55" s="94"/>
-      <c r="R55" s="62">
+      <c r="Q55" s="91"/>
+      <c r="R55" s="59">
         <f>IF(R43&gt;R44,R44,R43)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S55" s="91"/>
+      <c r="T55" s="59">
+        <f t="shared" ref="T55" si="33">IF(T43&gt;T44,T44,T43)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>59</v>
       </c>
       <c r="B56"/>
-      <c r="C56" s="62">
+      <c r="C56" s="59">
         <f>C54-C55</f>
         <v>1834</v>
       </c>
-      <c r="D56" s="62"/>
-      <c r="E56" s="62">
-        <f t="shared" ref="E56:K56" si="11">E54-E55</f>
+      <c r="D56" s="59"/>
+      <c r="E56" s="59">
+        <f t="shared" ref="E56:K56" si="34">E54-E55</f>
         <v>1196.5876623376626</v>
       </c>
-      <c r="F56" s="62"/>
-      <c r="G56" s="62">
-        <f t="shared" ref="G56" si="12">G54-G55</f>
-        <v>0</v>
-      </c>
-      <c r="H56" s="62"/>
-      <c r="I56" s="62">
-        <f t="shared" si="11"/>
+      <c r="F56" s="59"/>
+      <c r="G56" s="59">
+        <f t="shared" ref="G56" si="35">G54-G55</f>
+        <v>0</v>
+      </c>
+      <c r="H56" s="59"/>
+      <c r="I56" s="59">
+        <f t="shared" si="34"/>
         <v>122.99999999999999</v>
       </c>
-      <c r="J56" s="62"/>
-      <c r="K56" s="62">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="N56" s="62">
-        <f t="shared" ref="N56" si="13">N54-N55</f>
+      <c r="J56" s="59"/>
+      <c r="K56" s="59">
+        <f t="shared" si="34"/>
+        <v>122.99999999999999</v>
+      </c>
+      <c r="N56" s="59">
+        <f t="shared" ref="N56" si="36">N54-N55</f>
         <v>1186.9285714285716</v>
       </c>
-      <c r="O56" s="62"/>
-      <c r="P56" s="106">
-        <f t="shared" ref="P56" si="14">P54-P55</f>
+      <c r="O56" s="59"/>
+      <c r="P56" s="103">
+        <f t="shared" ref="P56" si="37">P54-P55</f>
         <v>1205.3999999999999</v>
       </c>
-      <c r="Q56" s="94"/>
-      <c r="R56" s="62">
-        <f t="shared" ref="R56" si="15">R54-R55</f>
+      <c r="Q56" s="91"/>
+      <c r="R56" s="59">
+        <f t="shared" ref="R56" si="38">R54-R55</f>
         <v>976.01298701298686</v>
       </c>
-      <c r="T56" s="48"/>
+      <c r="S56" s="91"/>
+      <c r="T56" s="59">
+        <f t="shared" ref="T56" si="39">T54-T55</f>
+        <v>1178.75</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="V57" s="108"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
@@ -3277,17 +3521,17 @@
       <c r="A17" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="51" t="s">
+      <c r="B17" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="52"/>
-      <c r="E17" s="51" t="s">
+      <c r="D17" s="51"/>
+      <c r="E17" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="F17" s="52"/>
+      <c r="F17" s="51"/>
       <c r="G17" s="11"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -3700,7 +3944,7 @@
       </c>
       <c r="F41" s="41"/>
       <c r="G41" s="42"/>
-      <c r="H41" s="53" t="s">
+      <c r="H41" s="52" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>